<commit_message>
test manager excel working
</commit_message>
<xml_diff>
--- a/recount/test/test_files/excel_input_1.xlsx
+++ b/recount/test/test_files/excel_input_1.xlsx
@@ -15,17 +15,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1645269141" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1645269141" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1645269141" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1645269141"/>
+      <pm:revision xmlns:pm="smNativeData" day="1666542496" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1666542496" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1666542496" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1666542496"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Currency</t>
+  </si>
+  <si>
+    <t>Receiver</t>
   </si>
   <si>
     <t>Description</t>
@@ -48,31 +51,40 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Type</t>
+    <t>Place</t>
   </si>
   <si>
-    <t>Travel</t>
+    <t>Payment Method</t>
   </si>
   <si>
     <t>EUR</t>
   </si>
   <si>
-    <t>Campus Laval  : 1er loyer du CAMPUS LAVAL</t>
+    <t>Campus Laval</t>
+  </si>
+  <si>
+    <t>1er loyer du CAMPUS LAVAL</t>
   </si>
   <si>
     <t>housing:rent</t>
   </si>
   <si>
+    <t>NY</t>
+  </si>
+  <si>
     <t>cash</t>
   </si>
   <si>
-    <t>NY</t>
+    <t>Air France</t>
   </si>
   <si>
     <t>Avion : billet France -&gt; Québec</t>
   </si>
   <si>
     <t>transport:plane</t>
+  </si>
+  <si>
+    <t>Fnac</t>
   </si>
   <si>
     <t>Equipement fnac, oreiller</t>
@@ -134,7 +146,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645269141" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1666542496" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -149,7 +161,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645269141" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1666542496" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -165,7 +177,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645269141" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1666542496" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -180,7 +192,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1645269141" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1666542496" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="240" lang="default"/>
             <pm:ea face="Basic Roman" sz="240" lang="default"/>
@@ -226,7 +238,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1645269141" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1666542496" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -248,7 +260,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1645269141"/>
+          <pm:border xmlns:pm="smNativeData" id="1666542496"/>
         </ext>
       </extLst>
     </border>
@@ -267,7 +279,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1645269141">
+          <pm:border xmlns:pm="smNativeData" id="1666542496">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -288,7 +300,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1645269141">
+          <pm:border xmlns:pm="smNativeData" id="1666542496">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -310,7 +322,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1645269141">
+          <pm:border xmlns:pm="smNativeData" id="1666542496">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -331,7 +343,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1645269141">
+          <pm:border xmlns:pm="smNativeData" id="1666542496">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -352,7 +364,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1645269141">
+          <pm:border xmlns:pm="smNativeData" id="1666542496">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -374,7 +386,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1645269141">
+          <pm:border xmlns:pm="smNativeData" id="1666542496">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -397,7 +409,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1645269141">
+          <pm:border xmlns:pm="smNativeData" id="1666542496">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -419,7 +431,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1645269141">
+          <pm:border xmlns:pm="smNativeData" id="1666542496">
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -440,7 +452,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1645269141"/>
+          <pm:border xmlns:pm="smNativeData" id="1666542496"/>
         </ext>
       </extLst>
     </border>
@@ -504,10 +516,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1645269141" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1666542496" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1645269141" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1666542496" count="1">
         <pm:color name="Gris 20%" rgb="000000"/>
       </pm:colors>
     </ext>
@@ -771,26 +783,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K624"/>
+  <dimension ref="A1:L624"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.553571" defaultRowHeight="15.40"/>
   <cols>
     <col min="2" max="2" width="17.553571" customWidth="1"/>
-    <col min="3" max="3" width="16.107143" customWidth="1"/>
-    <col min="4" max="4" width="51.330357" customWidth="1" style="8"/>
-    <col min="5" max="5" width="12.000000" customWidth="1" style="18"/>
-    <col min="6" max="6" width="21.258929" customWidth="1"/>
-    <col min="7" max="7" width="36.330357" customWidth="1" style="14"/>
+    <col min="3" max="4" width="16.107143" customWidth="1"/>
+    <col min="5" max="5" width="51.330357" customWidth="1" style="8"/>
+    <col min="6" max="6" width="12.000000" customWidth="1" style="18"/>
+    <col min="7" max="7" width="21.258929" customWidth="1"/>
+    <col min="8" max="8" width="36.330357" customWidth="1" style="14"/>
     <col min="9" max="9" width="18.437500" customWidth="1"/>
-    <col min="10" max="10" width="13.107143" customWidth="1"/>
-    <col min="11" max="11" width="14.000000" customWidth="1"/>
+    <col min="10" max="10" width="27.357143" customWidth="1"/>
+    <col min="11" max="11" width="18.437500" customWidth="1"/>
+    <col min="12" max="12" width="14.000000" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -800,26 +813,30 @@
       <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="17" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="n">
         <v>1</v>
       </c>
@@ -827,70 +844,81 @@
         <v>246.550000000000011</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="18" t="n">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="18" t="n">
         <v>43678</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
+      <c r="H2" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>545.230000000000018</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="K3"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="18" t="n">
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="18" t="n">
         <v>43681</v>
       </c>
-      <c r="G4" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
+      <c r="H4" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-    </row>
-    <row r="5" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4"/>
+      <c r="L4" s="12"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="n">
         <v>4</v>
       </c>
@@ -899,20 +927,21 @@
         <v>135</v>
       </c>
       <c r="C5"/>
-      <c r="D5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="18" t="n">
+      <c r="E5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="18" t="n">
         <v>43683</v>
       </c>
-      <c r="G5" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="H5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5"/>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="n">
         <v>5</v>
       </c>
@@ -920,25 +949,27 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="18" t="n">
+        <v>27</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6" s="18" t="n">
         <v>43687</v>
       </c>
-      <c r="G6" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" t="s">
-        <v>21</v>
+      <c r="H6" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="n">
         <v>6</v>
       </c>
@@ -947,16 +978,16 @@
       </c>
       <c r="C7"/>
       <c r="D7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="n">
-        <v>4</v>
-      </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>29</v>
+      </c>
+      <c r="E7"/>
+      <c r="G7"/>
+      <c r="I7"/>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="n">
         <v>7</v>
       </c>
@@ -964,29 +995,33 @@
         <v>30</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="18" t="n">
+        <v>31</v>
+      </c>
+      <c r="E8"/>
+      <c r="F8" s="18" t="n">
         <v>43692</v>
       </c>
-      <c r="G8" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="H8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8"/>
+      <c r="J8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9"/>
       <c r="B9" s="5"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" s="1"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11"/>
@@ -1003,17 +1038,19 @@
       <c r="B13" s="4"/>
       <c r="C13"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14"/>
       <c r="B14" s="5"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="10"/>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14" s="1"/>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="9"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16"/>
@@ -1055,17 +1092,19 @@
       <c r="B23" s="4"/>
       <c r="C23"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24"/>
       <c r="B24" s="5"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="10"/>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="D24" s="1"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="9"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26"/>
@@ -1092,29 +1131,33 @@
       <c r="B30" s="4"/>
       <c r="C30"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31"/>
       <c r="B31" s="5"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="10"/>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="D31" s="1"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32"/>
       <c r="B32" s="2"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="9"/>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="D32" s="3"/>
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33"/>
       <c r="B33" s="5"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="10"/>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="D33" s="1"/>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34"/>
       <c r="B34" s="2"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="9"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="9"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35"/>
@@ -1131,39 +1174,42 @@
       <c r="B37" s="4"/>
       <c r="C37"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="A38"/>
       <c r="B38" s="5"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="10"/>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="D38" s="1"/>
+      <c r="E38" s="10"/>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39"/>
       <c r="B39" s="2"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="9"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="9"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40"/>
       <c r="B40" s="4"/>
       <c r="C40"/>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:5">
       <c r="A41"/>
       <c r="B41" s="4"/>
       <c r="C41"/>
-      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42"/>
       <c r="B42" s="4"/>
       <c r="C42"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:5">
       <c r="A43"/>
       <c r="B43" s="2"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="9"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="9"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44"/>
@@ -1175,17 +1221,19 @@
       <c r="B45" s="4"/>
       <c r="C45"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:5">
       <c r="A46"/>
       <c r="B46" s="5"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="10"/>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="D46" s="1"/>
+      <c r="E46" s="10"/>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47"/>
       <c r="B47" s="2"/>
       <c r="C47" s="3"/>
-      <c r="D47" s="9"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="9"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48"/>
@@ -1212,17 +1260,19 @@
       <c r="B52" s="4"/>
       <c r="C52"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:5">
       <c r="A53"/>
       <c r="B53" s="5"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="10"/>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="D53" s="1"/>
+      <c r="E53" s="10"/>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54"/>
       <c r="B54" s="2"/>
       <c r="C54" s="3"/>
-      <c r="D54" s="9"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="9"/>
     </row>
     <row r="55" spans="1:3">
       <c r="A55"/>
@@ -1234,28 +1284,31 @@
       <c r="B56" s="4"/>
       <c r="C56"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:5">
       <c r="A57"/>
       <c r="B57" s="5"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="10"/>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="D57" s="1"/>
+      <c r="E57" s="10"/>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58"/>
       <c r="B58" s="2"/>
       <c r="C58" s="3"/>
-      <c r="D58" s="9"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="9"/>
     </row>
     <row r="59" spans="1:3">
       <c r="A59"/>
       <c r="B59" s="4"/>
       <c r="C59"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:5">
       <c r="A60"/>
       <c r="B60" s="6"/>
       <c r="C60" s="7"/>
-      <c r="D60" s="11"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="11"/>
     </row>
     <row r="61" spans="1:3">
       <c r="A61"/>
@@ -1267,29 +1320,33 @@
       <c r="B62" s="4"/>
       <c r="C62"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:5">
       <c r="A63"/>
       <c r="B63" s="5"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="10"/>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="D63" s="1"/>
+      <c r="E63" s="10"/>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64"/>
       <c r="B64" s="2"/>
       <c r="C64" s="3"/>
-      <c r="D64" s="9"/>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="D64" s="3"/>
+      <c r="E64" s="9"/>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65"/>
       <c r="B65" s="5"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="10"/>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="D65" s="1"/>
+      <c r="E65" s="10"/>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66"/>
       <c r="B66" s="2"/>
       <c r="C66" s="3"/>
-      <c r="D66" s="9"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="9"/>
     </row>
     <row r="67" spans="1:3">
       <c r="A67"/>
@@ -1306,70 +1363,80 @@
       <c r="B69" s="4"/>
       <c r="C69"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:5">
       <c r="A70"/>
       <c r="B70" s="5"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="10"/>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="D70" s="1"/>
+      <c r="E70" s="10"/>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71"/>
       <c r="B71" s="2"/>
       <c r="C71" s="3"/>
-      <c r="D71" s="9"/>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="D71" s="3"/>
+      <c r="E71" s="9"/>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72"/>
       <c r="B72" s="5"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="10"/>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="D72" s="1"/>
+      <c r="E72" s="10"/>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73"/>
       <c r="B73" s="2"/>
       <c r="C73" s="3"/>
-      <c r="D73" s="9"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="9"/>
     </row>
     <row r="74" spans="1:3">
       <c r="A74"/>
       <c r="B74" s="4"/>
       <c r="C74"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:5">
       <c r="A75"/>
       <c r="B75" s="5"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="10"/>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="D75" s="1"/>
+      <c r="E75" s="10"/>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76"/>
       <c r="B76" s="2"/>
       <c r="C76" s="3"/>
-      <c r="D76" s="9"/>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="D76" s="3"/>
+      <c r="E76" s="9"/>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77"/>
       <c r="B77" s="5"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="10"/>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="D77" s="1"/>
+      <c r="E77" s="10"/>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78"/>
       <c r="B78" s="2"/>
       <c r="C78" s="3"/>
-      <c r="D78" s="9"/>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="D78" s="3"/>
+      <c r="E78" s="9"/>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79"/>
       <c r="B79" s="5"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="10"/>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="D79" s="1"/>
+      <c r="E79" s="10"/>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80"/>
       <c r="B80" s="2"/>
       <c r="C80" s="3"/>
-      <c r="D80" s="9"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="9"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81"/>
@@ -1386,29 +1453,33 @@
       <c r="B83" s="4"/>
       <c r="C83"/>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:5">
       <c r="A84"/>
       <c r="B84" s="5"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="10"/>
-    </row>
-    <row r="85" spans="1:4">
+      <c r="D84" s="1"/>
+      <c r="E84" s="10"/>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85"/>
       <c r="B85" s="2"/>
       <c r="C85" s="3"/>
-      <c r="D85" s="9"/>
-    </row>
-    <row r="86" spans="1:4">
+      <c r="D85" s="3"/>
+      <c r="E85" s="9"/>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86"/>
       <c r="B86" s="5"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="10"/>
-    </row>
-    <row r="87" spans="1:4">
+      <c r="D86" s="1"/>
+      <c r="E86" s="10"/>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87"/>
       <c r="B87" s="2"/>
       <c r="C87" s="3"/>
-      <c r="D87" s="9"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="9"/>
     </row>
     <row r="88" spans="1:3">
       <c r="A88"/>
@@ -1440,75 +1511,85 @@
       <c r="B93" s="4"/>
       <c r="C93"/>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:5">
       <c r="A94"/>
       <c r="B94" s="5"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="10"/>
-    </row>
-    <row r="95" spans="1:4">
+      <c r="D94" s="1"/>
+      <c r="E94" s="10"/>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95"/>
       <c r="B95" s="2"/>
       <c r="C95" s="3"/>
-      <c r="D95" s="9"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="9"/>
     </row>
     <row r="96" spans="1:3">
       <c r="A96"/>
       <c r="B96" s="4"/>
       <c r="C96"/>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:5">
       <c r="A97"/>
       <c r="B97" s="5"/>
       <c r="C97" s="1"/>
-      <c r="D97" s="10"/>
-    </row>
-    <row r="98" spans="1:4">
+      <c r="D97" s="1"/>
+      <c r="E97" s="10"/>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98"/>
       <c r="B98" s="2"/>
       <c r="C98" s="3"/>
-      <c r="D98" s="9"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="9"/>
     </row>
     <row r="99" spans="1:3">
       <c r="A99"/>
       <c r="B99" s="4"/>
       <c r="C99"/>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:5">
       <c r="A100"/>
       <c r="B100" s="5"/>
       <c r="C100" s="1"/>
-      <c r="D100" s="10"/>
-    </row>
-    <row r="101" spans="1:4">
+      <c r="D100" s="1"/>
+      <c r="E100" s="10"/>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101"/>
       <c r="B101" s="2"/>
       <c r="C101" s="3"/>
-      <c r="D101" s="9"/>
-    </row>
-    <row r="102" spans="1:4">
+      <c r="D101" s="3"/>
+      <c r="E101" s="9"/>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102"/>
       <c r="B102" s="5"/>
       <c r="C102" s="1"/>
-      <c r="D102" s="10"/>
-    </row>
-    <row r="103" spans="1:4">
+      <c r="D102" s="1"/>
+      <c r="E102" s="10"/>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103"/>
       <c r="B103" s="2"/>
       <c r="C103" s="3"/>
-      <c r="D103" s="9"/>
-    </row>
-    <row r="104" spans="1:4">
+      <c r="D103" s="3"/>
+      <c r="E103" s="9"/>
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104"/>
       <c r="B104" s="5"/>
       <c r="C104" s="1"/>
-      <c r="D104" s="10"/>
-    </row>
-    <row r="105" spans="1:4">
+      <c r="D104" s="1"/>
+      <c r="E104" s="10"/>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105"/>
       <c r="B105" s="2"/>
       <c r="C105" s="3"/>
-      <c r="D105" s="9"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="9"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106"/>
@@ -1530,34 +1611,38 @@
       <c r="B109" s="4"/>
       <c r="C109"/>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:5">
       <c r="A110"/>
       <c r="B110" s="5"/>
       <c r="C110" s="1"/>
-      <c r="D110" s="10"/>
-    </row>
-    <row r="111" spans="1:4">
+      <c r="D110" s="1"/>
+      <c r="E110" s="10"/>
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111"/>
       <c r="B111" s="2"/>
       <c r="C111" s="3"/>
-      <c r="D111" s="9"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="9"/>
     </row>
     <row r="112" spans="1:3">
       <c r="A112"/>
       <c r="B112" s="4"/>
       <c r="C112"/>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:5">
       <c r="A113"/>
       <c r="B113" s="5"/>
       <c r="C113" s="1"/>
-      <c r="D113" s="10"/>
-    </row>
-    <row r="114" spans="1:4">
+      <c r="D113" s="1"/>
+      <c r="E113" s="10"/>
+    </row>
+    <row r="114" spans="1:5">
       <c r="A114"/>
       <c r="B114" s="2"/>
       <c r="C114" s="3"/>
-      <c r="D114" s="9"/>
+      <c r="D114" s="3"/>
+      <c r="E114" s="9"/>
     </row>
     <row r="115" spans="1:3">
       <c r="A115"/>
@@ -1583,35 +1668,37 @@
       <c r="A119"/>
       <c r="B119" s="4"/>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:5">
       <c r="A120"/>
       <c r="B120" s="3"/>
-      <c r="D120" s="9"/>
+      <c r="E120" s="9"/>
     </row>
     <row r="121" spans="1:2">
       <c r="A121"/>
       <c r="B121"/>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:7">
       <c r="A122"/>
       <c r="B122"/>
-      <c r="F122"/>
-    </row>
-    <row r="123" spans="1:6">
+      <c r="G122"/>
+    </row>
+    <row r="123" spans="1:7">
       <c r="A123"/>
       <c r="B123"/>
-      <c r="F123"/>
-    </row>
-    <row r="124" spans="1:3">
+      <c r="G123"/>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124"/>
       <c r="B124" s="5"/>
       <c r="C124" s="1"/>
-    </row>
-    <row r="125" spans="1:4">
+      <c r="D124" s="1"/>
+    </row>
+    <row r="125" spans="1:5">
       <c r="A125"/>
       <c r="B125" s="2"/>
       <c r="C125" s="3"/>
-      <c r="D125" s="9"/>
+      <c r="D125" s="3"/>
+      <c r="E125" s="9"/>
     </row>
     <row r="126" spans="1:3">
       <c r="A126"/>
@@ -1633,57 +1720,65 @@
       <c r="B129" s="4"/>
       <c r="C129"/>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:5">
       <c r="A130"/>
       <c r="B130" s="5"/>
       <c r="C130" s="1"/>
-      <c r="D130" s="10"/>
-    </row>
-    <row r="131" spans="1:4">
+      <c r="D130" s="1"/>
+      <c r="E130" s="10"/>
+    </row>
+    <row r="131" spans="1:5">
       <c r="A131"/>
       <c r="B131" s="2"/>
       <c r="C131" s="3"/>
-      <c r="D131" s="9"/>
-    </row>
-    <row r="132" spans="1:4">
+      <c r="D131" s="3"/>
+      <c r="E131" s="9"/>
+    </row>
+    <row r="132" spans="1:5">
       <c r="A132"/>
       <c r="B132" s="5"/>
       <c r="C132" s="1"/>
-      <c r="D132" s="10"/>
-    </row>
-    <row r="133" spans="1:4">
+      <c r="D132" s="1"/>
+      <c r="E132" s="10"/>
+    </row>
+    <row r="133" spans="1:5">
       <c r="A133"/>
       <c r="B133" s="2"/>
       <c r="C133" s="3"/>
-      <c r="D133" s="9"/>
-    </row>
-    <row r="134" spans="1:4">
+      <c r="D133" s="3"/>
+      <c r="E133" s="9"/>
+    </row>
+    <row r="134" spans="1:5">
       <c r="A134"/>
       <c r="B134" s="5"/>
       <c r="C134" s="1"/>
-      <c r="D134" s="10"/>
-    </row>
-    <row r="135" spans="1:4">
+      <c r="D134" s="1"/>
+      <c r="E134" s="10"/>
+    </row>
+    <row r="135" spans="1:5">
       <c r="A135"/>
       <c r="B135" s="2"/>
       <c r="C135" s="3"/>
-      <c r="D135" s="9"/>
-    </row>
-    <row r="136" spans="1:9">
+      <c r="D135" s="3"/>
+      <c r="E135" s="9"/>
+    </row>
+    <row r="136" spans="1:10">
       <c r="A136"/>
       <c r="B136" s="4"/>
       <c r="C136"/>
       <c r="I136"/>
+      <c r="J136"/>
     </row>
     <row r="137" spans="1:2">
       <c r="A137"/>
       <c r="B137" s="4"/>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:5">
       <c r="A138"/>
       <c r="B138" s="6"/>
       <c r="C138" s="7"/>
-      <c r="D138" s="11"/>
+      <c r="D138" s="7"/>
+      <c r="E138" s="11"/>
     </row>
     <row r="139" spans="1:3">
       <c r="A139"/>
@@ -1695,73 +1790,83 @@
       <c r="B140" s="4"/>
       <c r="C140"/>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:5">
       <c r="A141"/>
       <c r="B141" s="5"/>
       <c r="C141" s="1"/>
-      <c r="D141" s="10"/>
-    </row>
-    <row r="142" spans="1:4">
+      <c r="D141" s="1"/>
+      <c r="E141" s="10"/>
+    </row>
+    <row r="142" spans="1:5">
       <c r="A142"/>
       <c r="B142" s="2"/>
       <c r="C142" s="3"/>
-      <c r="D142" s="9"/>
+      <c r="D142" s="3"/>
+      <c r="E142" s="9"/>
     </row>
     <row r="143" spans="1:3">
       <c r="A143"/>
       <c r="B143" s="4"/>
       <c r="C143"/>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:5">
       <c r="A144"/>
       <c r="B144" s="5"/>
       <c r="C144" s="1"/>
-      <c r="D144" s="10"/>
-    </row>
-    <row r="145" spans="1:4">
+      <c r="D144" s="1"/>
+      <c r="E144" s="10"/>
+    </row>
+    <row r="145" spans="1:5">
       <c r="A145"/>
       <c r="B145" s="2"/>
       <c r="C145" s="3"/>
-      <c r="D145" s="9"/>
+      <c r="D145" s="3"/>
+      <c r="E145" s="9"/>
     </row>
     <row r="146" spans="1:3">
       <c r="A146"/>
       <c r="B146" s="4"/>
       <c r="C146"/>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:5">
       <c r="A147"/>
       <c r="B147" s="5"/>
       <c r="C147" s="1"/>
-      <c r="D147" s="10"/>
-    </row>
-    <row r="148" spans="1:4">
+      <c r="D147" s="1"/>
+      <c r="E147" s="10"/>
+    </row>
+    <row r="148" spans="1:5">
       <c r="A148"/>
       <c r="B148" s="2"/>
       <c r="C148" s="3"/>
-      <c r="D148" s="9"/>
-    </row>
-    <row r="149" spans="1:4">
+      <c r="D148" s="3"/>
+      <c r="E148" s="9"/>
+    </row>
+    <row r="149" spans="1:5">
       <c r="A149"/>
       <c r="B149" s="5"/>
       <c r="C149" s="1"/>
-      <c r="D149" s="10"/>
-    </row>
-    <row r="150" spans="1:4">
+      <c r="D149" s="1"/>
+      <c r="E149" s="10"/>
+    </row>
+    <row r="150" spans="1:5">
       <c r="A150"/>
       <c r="B150" s="2"/>
       <c r="C150" s="3"/>
-      <c r="D150" s="9"/>
-    </row>
-    <row r="151" spans="1:9">
+      <c r="D150" s="3"/>
+      <c r="E150" s="9"/>
+    </row>
+    <row r="151" spans="1:10">
       <c r="A151"/>
       <c r="B151" s="4"/>
       <c r="I151"/>
-    </row>
-    <row r="152" spans="1:9">
+      <c r="J151"/>
+    </row>
+    <row r="152" spans="1:10">
       <c r="A152"/>
       <c r="B152" s="4"/>
       <c r="I152"/>
+      <c r="J152"/>
     </row>
     <row r="153" spans="1:2">
       <c r="A153"/>
@@ -1771,11 +1876,12 @@
       <c r="A154"/>
       <c r="B154" s="4"/>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:5">
       <c r="A155"/>
       <c r="B155" s="2"/>
       <c r="C155" s="3"/>
-      <c r="D155" s="9"/>
+      <c r="D155" s="3"/>
+      <c r="E155" s="9"/>
     </row>
     <row r="156" spans="1:3">
       <c r="A156"/>
@@ -1790,55 +1896,62 @@
       <c r="A158"/>
       <c r="B158" s="4"/>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:5">
       <c r="A159"/>
       <c r="B159" s="5"/>
       <c r="C159" s="1"/>
-      <c r="D159" s="10"/>
+      <c r="D159" s="1"/>
+      <c r="E159" s="10"/>
     </row>
     <row r="160" spans="1:3">
       <c r="A160"/>
       <c r="B160" s="4"/>
       <c r="C160"/>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:5">
       <c r="A161"/>
       <c r="B161" s="5"/>
       <c r="C161" s="1"/>
-      <c r="D161" s="10"/>
-    </row>
-    <row r="162" spans="1:4">
+      <c r="D161" s="1"/>
+      <c r="E161" s="10"/>
+    </row>
+    <row r="162" spans="1:5">
       <c r="A162"/>
       <c r="B162" s="2"/>
       <c r="C162" s="3"/>
-      <c r="D162" s="9"/>
-    </row>
-    <row r="163" spans="1:4">
+      <c r="D162" s="3"/>
+      <c r="E162" s="9"/>
+    </row>
+    <row r="163" spans="1:5">
       <c r="A163"/>
       <c r="B163" s="5"/>
       <c r="C163" s="1"/>
-      <c r="D163" s="10"/>
-    </row>
-    <row r="164" spans="1:4">
+      <c r="D163" s="1"/>
+      <c r="E163" s="10"/>
+    </row>
+    <row r="164" spans="1:5">
       <c r="A164"/>
       <c r="B164" s="2"/>
       <c r="C164" s="3"/>
-      <c r="D164" s="9"/>
-    </row>
-    <row r="165" spans="1:9">
+      <c r="D164" s="3"/>
+      <c r="E164" s="9"/>
+    </row>
+    <row r="165" spans="1:10">
       <c r="A165"/>
       <c r="B165" s="4"/>
       <c r="I165"/>
+      <c r="J165"/>
     </row>
     <row r="166" spans="1:2">
       <c r="A166"/>
       <c r="B166" s="4"/>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:5">
       <c r="A167"/>
       <c r="B167" s="2"/>
       <c r="C167" s="3"/>
-      <c r="D167" s="9"/>
+      <c r="D167" s="3"/>
+      <c r="E167" s="9"/>
     </row>
     <row r="168" spans="1:3">
       <c r="A168"/>
@@ -1849,105 +1962,126 @@
       <c r="A169"/>
       <c r="B169" s="4"/>
     </row>
-    <row r="170" spans="1:9">
+    <row r="170" spans="1:10">
       <c r="A170"/>
       <c r="B170" s="2"/>
       <c r="C170" s="3"/>
-      <c r="D170" s="9"/>
+      <c r="D170" s="3"/>
+      <c r="E170" s="9"/>
       <c r="I170"/>
-    </row>
-    <row r="171" spans="1:9">
+      <c r="J170"/>
+    </row>
+    <row r="171" spans="1:10">
       <c r="A171"/>
       <c r="B171" s="4"/>
       <c r="I171"/>
-    </row>
-    <row r="172" spans="1:9">
+      <c r="J171"/>
+    </row>
+    <row r="172" spans="1:10">
       <c r="A172"/>
       <c r="B172" s="4"/>
       <c r="I172"/>
-    </row>
-    <row r="173" spans="1:9">
+      <c r="J172"/>
+    </row>
+    <row r="173" spans="1:10">
       <c r="A173"/>
       <c r="B173" s="4"/>
       <c r="I173"/>
-    </row>
-    <row r="174" spans="1:4">
+      <c r="J173"/>
+    </row>
+    <row r="174" spans="1:5">
       <c r="A174"/>
       <c r="B174" s="5"/>
       <c r="C174" s="1"/>
-      <c r="D174" s="10"/>
-    </row>
-    <row r="175" spans="1:9">
+      <c r="D174" s="1"/>
+      <c r="E174" s="10"/>
+    </row>
+    <row r="175" spans="1:10">
       <c r="A175"/>
       <c r="B175" s="4"/>
       <c r="I175"/>
-    </row>
-    <row r="176" spans="1:9">
+      <c r="J175"/>
+    </row>
+    <row r="176" spans="1:10">
       <c r="A176"/>
       <c r="B176" s="4"/>
       <c r="I176"/>
-    </row>
-    <row r="177" spans="1:9">
+      <c r="J176"/>
+    </row>
+    <row r="177" spans="1:10">
       <c r="A177"/>
       <c r="B177" s="4"/>
       <c r="I177"/>
-    </row>
-    <row r="178" spans="1:9">
+      <c r="J177"/>
+    </row>
+    <row r="178" spans="1:10">
       <c r="A178"/>
       <c r="B178" s="4"/>
       <c r="I178"/>
-    </row>
-    <row r="179" spans="1:9">
+      <c r="J178"/>
+    </row>
+    <row r="179" spans="1:10">
       <c r="A179"/>
       <c r="B179" s="4"/>
       <c r="I179"/>
-    </row>
-    <row r="180" spans="1:4">
+      <c r="J179"/>
+    </row>
+    <row r="180" spans="1:5">
       <c r="A180"/>
       <c r="B180" s="5"/>
       <c r="C180" s="1"/>
-      <c r="D180" s="10"/>
-    </row>
-    <row r="181" spans="1:9">
+      <c r="D180" s="1"/>
+      <c r="E180" s="10"/>
+    </row>
+    <row r="181" spans="1:10">
       <c r="A181"/>
       <c r="B181" s="2"/>
       <c r="C181" s="3"/>
-      <c r="D181" s="9"/>
+      <c r="D181" s="3"/>
+      <c r="E181" s="9"/>
       <c r="I181"/>
-    </row>
-    <row r="182" spans="1:9">
+      <c r="J181"/>
+    </row>
+    <row r="182" spans="1:10">
       <c r="A182"/>
       <c r="B182" s="4"/>
       <c r="I182"/>
-    </row>
-    <row r="183" spans="1:9">
+      <c r="J182"/>
+    </row>
+    <row r="183" spans="1:10">
       <c r="A183"/>
       <c r="B183" s="4"/>
       <c r="I183"/>
-    </row>
-    <row r="184" spans="1:4">
+      <c r="J183"/>
+    </row>
+    <row r="184" spans="1:5">
       <c r="A184"/>
       <c r="B184" s="5"/>
       <c r="C184" s="1"/>
-      <c r="D184" s="10"/>
-    </row>
-    <row r="185" spans="1:9">
+      <c r="D184" s="1"/>
+      <c r="E184" s="10"/>
+    </row>
+    <row r="185" spans="1:10">
       <c r="A185"/>
       <c r="B185" s="2"/>
       <c r="C185" s="3"/>
-      <c r="D185" s="9"/>
+      <c r="D185" s="3"/>
+      <c r="E185" s="9"/>
       <c r="I185"/>
-    </row>
-    <row r="186" spans="1:9">
+      <c r="J185"/>
+    </row>
+    <row r="186" spans="1:10">
       <c r="A186"/>
       <c r="B186" s="4"/>
       <c r="I186"/>
-    </row>
-    <row r="187" spans="1:4">
+      <c r="J186"/>
+    </row>
+    <row r="187" spans="1:5">
       <c r="A187"/>
       <c r="B187" s="5"/>
       <c r="C187" s="1"/>
-      <c r="D187" s="10"/>
+      <c r="D187" s="1"/>
+      <c r="E187" s="10"/>
     </row>
     <row r="188" spans="1:2">
       <c r="A188"/>
@@ -1958,45 +2092,50 @@
       <c r="B189" s="4"/>
       <c r="C189"/>
     </row>
-    <row r="190" spans="1:4">
+    <row r="190" spans="1:5">
       <c r="A190"/>
       <c r="B190" s="5"/>
       <c r="C190" s="1"/>
-      <c r="D190" s="10"/>
-    </row>
-    <row r="191" spans="1:4">
+      <c r="D190" s="1"/>
+      <c r="E190" s="10"/>
+    </row>
+    <row r="191" spans="1:5">
       <c r="A191"/>
       <c r="B191" s="2"/>
       <c r="C191" s="3"/>
-      <c r="D191" s="9"/>
+      <c r="D191" s="3"/>
+      <c r="E191" s="9"/>
     </row>
     <row r="192" spans="1:3">
       <c r="A192"/>
       <c r="B192" s="4"/>
       <c r="C192"/>
     </row>
-    <row r="193" spans="1:4">
+    <row r="193" spans="1:5">
       <c r="A193"/>
       <c r="B193" s="5"/>
       <c r="C193" s="1"/>
-      <c r="D193" s="10"/>
-    </row>
-    <row r="194" spans="1:4">
+      <c r="D193" s="1"/>
+      <c r="E193" s="10"/>
+    </row>
+    <row r="194" spans="1:5">
       <c r="A194"/>
       <c r="B194" s="2"/>
       <c r="C194" s="3"/>
-      <c r="D194" s="9"/>
+      <c r="D194" s="3"/>
+      <c r="E194" s="9"/>
     </row>
     <row r="195" spans="1:3">
       <c r="A195"/>
       <c r="B195" s="4"/>
       <c r="C195"/>
     </row>
-    <row r="196" spans="1:4">
+    <row r="196" spans="1:5">
       <c r="A196"/>
       <c r="B196" s="5"/>
       <c r="C196" s="1"/>
-      <c r="D196" s="10"/>
+      <c r="D196" s="1"/>
+      <c r="E196" s="10"/>
     </row>
     <row r="197" spans="1:1">
       <c r="A197"/>
@@ -2008,10 +2147,11 @@
     <row r="199" spans="1:1">
       <c r="A199"/>
     </row>
-    <row r="200" spans="1:9">
+    <row r="200" spans="1:10">
       <c r="A200"/>
       <c r="B200"/>
       <c r="I200"/>
+      <c r="J200"/>
     </row>
     <row r="201" spans="1:1">
       <c r="A201"/>
@@ -2025,120 +2165,141 @@
     <row r="204" spans="1:1">
       <c r="A204"/>
     </row>
-    <row r="205" spans="1:9">
+    <row r="205" spans="1:10">
       <c r="A205"/>
       <c r="B205" s="2"/>
       <c r="C205" s="3"/>
-      <c r="D205" s="9"/>
+      <c r="D205" s="3"/>
+      <c r="E205" s="9"/>
       <c r="I205"/>
-    </row>
-    <row r="206" spans="1:4">
+      <c r="J205"/>
+    </row>
+    <row r="206" spans="1:5">
       <c r="A206"/>
       <c r="B206" s="5"/>
       <c r="C206" s="1"/>
-      <c r="D206" s="10"/>
-    </row>
-    <row r="207" spans="1:9">
+      <c r="D206" s="1"/>
+      <c r="E206" s="10"/>
+    </row>
+    <row r="207" spans="1:10">
       <c r="A207"/>
       <c r="B207" s="2"/>
       <c r="C207" s="3"/>
-      <c r="D207" s="9"/>
+      <c r="D207" s="3"/>
+      <c r="E207" s="9"/>
       <c r="I207"/>
-    </row>
-    <row r="208" spans="1:4">
+      <c r="J207"/>
+    </row>
+    <row r="208" spans="1:5">
       <c r="A208"/>
       <c r="B208" s="5"/>
       <c r="C208" s="1"/>
-      <c r="D208" s="10"/>
-    </row>
-    <row r="209" spans="1:9">
+      <c r="D208" s="1"/>
+      <c r="E208" s="10"/>
+    </row>
+    <row r="209" spans="1:10">
       <c r="A209"/>
       <c r="B209" s="2"/>
       <c r="C209" s="3"/>
-      <c r="D209" s="9"/>
+      <c r="D209" s="3"/>
+      <c r="E209" s="9"/>
       <c r="I209"/>
-    </row>
-    <row r="210" spans="1:4">
+      <c r="J209"/>
+    </row>
+    <row r="210" spans="1:5">
       <c r="A210"/>
       <c r="B210" s="5"/>
       <c r="C210" s="1"/>
-      <c r="D210" s="10"/>
-    </row>
-    <row r="211" spans="1:9">
+      <c r="D210" s="1"/>
+      <c r="E210" s="10"/>
+    </row>
+    <row r="211" spans="1:10">
       <c r="A211"/>
       <c r="B211" s="2"/>
       <c r="C211" s="3"/>
-      <c r="D211" s="9"/>
+      <c r="D211" s="3"/>
+      <c r="E211" s="9"/>
       <c r="I211"/>
-    </row>
-    <row r="212" spans="1:4">
+      <c r="J211"/>
+    </row>
+    <row r="212" spans="1:5">
       <c r="A212"/>
       <c r="B212" s="5"/>
       <c r="C212" s="1"/>
-      <c r="D212" s="10"/>
-    </row>
-    <row r="213" spans="1:4">
+      <c r="D212" s="1"/>
+      <c r="E212" s="10"/>
+    </row>
+    <row r="213" spans="1:5">
       <c r="A213"/>
       <c r="B213" s="2"/>
       <c r="C213" s="3"/>
-      <c r="D213" s="9"/>
+      <c r="D213" s="3"/>
+      <c r="E213" s="9"/>
     </row>
     <row r="214" spans="1:2">
       <c r="A214"/>
       <c r="B214" s="4"/>
     </row>
-    <row r="215" spans="1:4">
+    <row r="215" spans="1:5">
       <c r="A215"/>
       <c r="B215" s="5"/>
       <c r="C215" s="1"/>
-      <c r="D215" s="10"/>
-    </row>
-    <row r="216" spans="1:4">
+      <c r="D215" s="1"/>
+      <c r="E215" s="10"/>
+    </row>
+    <row r="216" spans="1:5">
       <c r="A216"/>
       <c r="B216" s="2"/>
       <c r="C216" s="3"/>
-      <c r="D216" s="9"/>
+      <c r="D216" s="3"/>
+      <c r="E216" s="9"/>
     </row>
     <row r="217" spans="1:3">
       <c r="A217"/>
       <c r="B217" s="4"/>
       <c r="C217"/>
     </row>
-    <row r="218" spans="1:4">
+    <row r="218" spans="1:5">
       <c r="A218"/>
       <c r="B218" s="5"/>
       <c r="C218" s="1"/>
-      <c r="D218" s="10"/>
-    </row>
-    <row r="219" spans="1:4">
+      <c r="D218" s="1"/>
+      <c r="E218" s="10"/>
+    </row>
+    <row r="219" spans="1:5">
       <c r="A219"/>
       <c r="B219" s="2"/>
       <c r="C219" s="3"/>
-      <c r="D219" s="9"/>
-    </row>
-    <row r="220" spans="1:4">
+      <c r="D219" s="3"/>
+      <c r="E219" s="9"/>
+    </row>
+    <row r="220" spans="1:5">
       <c r="A220"/>
       <c r="B220" s="5"/>
       <c r="C220" s="1"/>
-      <c r="D220" s="10"/>
-    </row>
-    <row r="221" spans="1:4">
+      <c r="D220" s="1"/>
+      <c r="E220" s="10"/>
+    </row>
+    <row r="221" spans="1:5">
       <c r="A221"/>
       <c r="B221" s="2"/>
       <c r="C221" s="3"/>
-      <c r="D221" s="9"/>
-    </row>
-    <row r="222" spans="1:4">
+      <c r="D221" s="3"/>
+      <c r="E221" s="9"/>
+    </row>
+    <row r="222" spans="1:5">
       <c r="A222"/>
       <c r="B222" s="5"/>
       <c r="C222" s="1"/>
-      <c r="D222" s="10"/>
-    </row>
-    <row r="223" spans="1:4">
+      <c r="D222" s="1"/>
+      <c r="E222" s="10"/>
+    </row>
+    <row r="223" spans="1:5">
       <c r="A223"/>
       <c r="B223" s="2"/>
       <c r="C223" s="3"/>
-      <c r="D223" s="9"/>
+      <c r="D223" s="3"/>
+      <c r="E223" s="9"/>
     </row>
     <row r="224" spans="1:3">
       <c r="A224"/>
@@ -2155,34 +2316,38 @@
       <c r="B226" s="4"/>
       <c r="C226"/>
     </row>
-    <row r="227" spans="1:4">
+    <row r="227" spans="1:5">
       <c r="A227"/>
       <c r="B227" s="5"/>
       <c r="C227" s="1"/>
-      <c r="D227" s="10"/>
-    </row>
-    <row r="228" spans="1:4">
+      <c r="D227" s="1"/>
+      <c r="E227" s="10"/>
+    </row>
+    <row r="228" spans="1:5">
       <c r="A228"/>
       <c r="B228" s="2"/>
       <c r="C228" s="3"/>
-      <c r="D228" s="9"/>
+      <c r="D228" s="3"/>
+      <c r="E228" s="9"/>
     </row>
     <row r="229" spans="1:3">
       <c r="A229"/>
       <c r="B229" s="4"/>
       <c r="C229"/>
     </row>
-    <row r="230" spans="1:4">
+    <row r="230" spans="1:5">
       <c r="A230"/>
       <c r="B230" s="5"/>
       <c r="C230" s="1"/>
-      <c r="D230" s="10"/>
-    </row>
-    <row r="231" spans="1:4">
+      <c r="D230" s="1"/>
+      <c r="E230" s="10"/>
+    </row>
+    <row r="231" spans="1:5">
       <c r="A231"/>
       <c r="B231" s="2"/>
       <c r="C231" s="3"/>
-      <c r="D231" s="9"/>
+      <c r="D231" s="3"/>
+      <c r="E231" s="9"/>
     </row>
     <row r="232" spans="1:3">
       <c r="A232"/>
@@ -2194,49 +2359,57 @@
       <c r="B233" s="4"/>
       <c r="C233"/>
     </row>
-    <row r="234" spans="1:4">
+    <row r="234" spans="1:5">
       <c r="A234"/>
       <c r="B234" s="5"/>
       <c r="C234" s="1"/>
-      <c r="D234" s="10"/>
-    </row>
-    <row r="235" spans="1:9">
+      <c r="D234" s="1"/>
+      <c r="E234" s="10"/>
+    </row>
+    <row r="235" spans="1:10">
       <c r="A235"/>
       <c r="B235" s="2"/>
       <c r="C235" s="3"/>
-      <c r="D235" s="9"/>
+      <c r="D235" s="3"/>
+      <c r="E235" s="9"/>
       <c r="I235"/>
-    </row>
-    <row r="236" spans="1:9">
+      <c r="J235"/>
+    </row>
+    <row r="236" spans="1:10">
       <c r="A236"/>
       <c r="B236" s="4"/>
       <c r="C236"/>
       <c r="I236"/>
-    </row>
-    <row r="237" spans="1:9">
+      <c r="J236"/>
+    </row>
+    <row r="237" spans="1:10">
       <c r="A237"/>
       <c r="B237" s="4"/>
       <c r="C237"/>
-      <c r="F237"/>
+      <c r="G237"/>
       <c r="I237"/>
-    </row>
-    <row r="238" spans="1:9">
+      <c r="J237"/>
+    </row>
+    <row r="238" spans="1:10">
       <c r="A238"/>
       <c r="B238" s="4"/>
       <c r="C238"/>
       <c r="I238"/>
-    </row>
-    <row r="239" spans="1:4">
+      <c r="J238"/>
+    </row>
+    <row r="239" spans="1:5">
       <c r="A239"/>
       <c r="B239" s="5"/>
       <c r="C239" s="1"/>
-      <c r="D239" s="10"/>
-    </row>
-    <row r="240" spans="1:4">
+      <c r="D239" s="1"/>
+      <c r="E239" s="10"/>
+    </row>
+    <row r="240" spans="1:5">
       <c r="A240"/>
       <c r="B240" s="2"/>
       <c r="C240" s="3"/>
-      <c r="D240" s="9"/>
+      <c r="D240" s="3"/>
+      <c r="E240" s="9"/>
     </row>
     <row r="241" spans="1:3">
       <c r="A241"/>
@@ -2257,17 +2430,19 @@
       <c r="B244" s="4"/>
       <c r="C244"/>
     </row>
-    <row r="245" spans="1:4">
+    <row r="245" spans="1:5">
       <c r="A245"/>
       <c r="B245" s="5"/>
       <c r="C245" s="1"/>
-      <c r="D245" s="10"/>
-    </row>
-    <row r="246" spans="1:4">
+      <c r="D245" s="1"/>
+      <c r="E245" s="10"/>
+    </row>
+    <row r="246" spans="1:5">
       <c r="A246"/>
       <c r="B246" s="2"/>
       <c r="C246" s="3"/>
-      <c r="D246" s="9"/>
+      <c r="D246" s="3"/>
+      <c r="E246" s="9"/>
     </row>
     <row r="247" spans="1:3">
       <c r="A247"/>
@@ -2278,90 +2453,100 @@
       <c r="A248"/>
       <c r="B248" s="4"/>
     </row>
-    <row r="249" spans="1:4">
+    <row r="249" spans="1:5">
       <c r="A249"/>
       <c r="B249" s="6"/>
       <c r="C249" s="7"/>
-      <c r="D249" s="11"/>
+      <c r="D249" s="7"/>
+      <c r="E249" s="11"/>
     </row>
     <row r="250" spans="1:3">
       <c r="A250"/>
       <c r="B250" s="4"/>
       <c r="C250"/>
     </row>
-    <row r="251" spans="1:4">
+    <row r="251" spans="1:5">
       <c r="A251"/>
       <c r="B251" s="5"/>
       <c r="C251" s="1"/>
-      <c r="D251" s="10"/>
-    </row>
-    <row r="252" spans="1:4">
+      <c r="D251" s="1"/>
+      <c r="E251" s="10"/>
+    </row>
+    <row r="252" spans="1:5">
       <c r="A252"/>
       <c r="B252" s="2"/>
       <c r="C252" s="3"/>
-      <c r="D252" s="9"/>
+      <c r="D252" s="3"/>
+      <c r="E252" s="9"/>
     </row>
     <row r="253" spans="1:3">
       <c r="A253"/>
       <c r="B253" s="4"/>
       <c r="C253"/>
     </row>
-    <row r="254" spans="1:4">
+    <row r="254" spans="1:5">
       <c r="A254"/>
       <c r="B254" s="5"/>
       <c r="C254" s="1"/>
-      <c r="D254" s="10"/>
-    </row>
-    <row r="255" spans="1:4">
+      <c r="D254" s="1"/>
+      <c r="E254" s="10"/>
+    </row>
+    <row r="255" spans="1:5">
       <c r="A255"/>
       <c r="B255" s="2"/>
       <c r="C255" s="3"/>
-      <c r="D255" s="9"/>
-    </row>
-    <row r="256" spans="1:6">
+      <c r="D255" s="3"/>
+      <c r="E255" s="9"/>
+    </row>
+    <row r="256" spans="1:7">
       <c r="A256"/>
       <c r="B256" s="4"/>
       <c r="C256"/>
-      <c r="F256"/>
+      <c r="G256"/>
     </row>
     <row r="257" spans="1:3">
       <c r="A257"/>
       <c r="B257" s="4"/>
       <c r="C257"/>
     </row>
-    <row r="258" spans="1:4">
+    <row r="258" spans="1:5">
       <c r="A258"/>
       <c r="B258" s="5"/>
       <c r="C258" s="1"/>
-      <c r="D258" s="10"/>
-    </row>
-    <row r="259" spans="1:4">
+      <c r="D258" s="1"/>
+      <c r="E258" s="10"/>
+    </row>
+    <row r="259" spans="1:5">
       <c r="A259"/>
       <c r="B259" s="2"/>
       <c r="C259" s="3"/>
-      <c r="D259" s="9"/>
-    </row>
-    <row r="260" spans="1:4">
+      <c r="D259" s="3"/>
+      <c r="E259" s="9"/>
+    </row>
+    <row r="260" spans="1:5">
       <c r="A260"/>
       <c r="B260" s="5"/>
       <c r="C260" s="1"/>
-      <c r="D260" s="10"/>
-    </row>
-    <row r="261" spans="1:4">
+      <c r="D260" s="1"/>
+      <c r="E260" s="10"/>
+    </row>
+    <row r="261" spans="1:5">
       <c r="A261"/>
       <c r="B261" s="2"/>
       <c r="C261" s="3"/>
-      <c r="D261" s="9"/>
+      <c r="D261" s="3"/>
+      <c r="E261" s="9"/>
     </row>
     <row r="262" spans="1:2">
       <c r="A262"/>
       <c r="B262" s="4"/>
     </row>
-    <row r="263" spans="1:4">
+    <row r="263" spans="1:5">
       <c r="A263"/>
       <c r="B263" s="2"/>
       <c r="C263" s="3"/>
-      <c r="D263" s="9"/>
+      <c r="D263" s="3"/>
+      <c r="E263" s="9"/>
     </row>
     <row r="264" spans="1:3">
       <c r="A264"/>
@@ -2377,11 +2562,12 @@
       <c r="A266"/>
       <c r="B266" s="4"/>
     </row>
-    <row r="267" spans="1:4">
+    <row r="267" spans="1:5">
       <c r="A267"/>
       <c r="B267" s="2"/>
       <c r="C267" s="3"/>
-      <c r="D267" s="9"/>
+      <c r="D267" s="3"/>
+      <c r="E267" s="9"/>
     </row>
     <row r="268" spans="1:3">
       <c r="A268"/>
@@ -2392,64 +2578,68 @@
       <c r="A269"/>
       <c r="B269" s="4"/>
     </row>
-    <row r="270" spans="1:4">
+    <row r="270" spans="1:5">
       <c r="A270"/>
       <c r="B270" s="2"/>
       <c r="C270" s="3"/>
-      <c r="D270" s="9"/>
-    </row>
-    <row r="271" spans="1:4">
+      <c r="D270" s="3"/>
+      <c r="E270" s="9"/>
+    </row>
+    <row r="271" spans="1:5">
       <c r="A271"/>
       <c r="B271" s="4"/>
       <c r="C271"/>
-      <c r="D271"/>
+      <c r="E271"/>
     </row>
     <row r="272" spans="1:3">
       <c r="A272"/>
       <c r="B272" s="4"/>
       <c r="C272"/>
     </row>
-    <row r="273" spans="1:6">
+    <row r="273" spans="1:7">
       <c r="A273"/>
       <c r="B273" s="4"/>
       <c r="C273"/>
-      <c r="F273"/>
+      <c r="G273"/>
     </row>
     <row r="274" spans="1:2">
       <c r="A274"/>
       <c r="B274" s="4"/>
     </row>
-    <row r="275" spans="1:4">
+    <row r="275" spans="1:5">
       <c r="A275"/>
       <c r="B275" s="2"/>
       <c r="C275" s="3"/>
-      <c r="D275" s="9"/>
+      <c r="D275" s="3"/>
+      <c r="E275" s="9"/>
     </row>
     <row r="276" spans="1:2">
       <c r="A276"/>
       <c r="B276" s="4"/>
     </row>
-    <row r="277" spans="1:4">
+    <row r="277" spans="1:5">
       <c r="A277"/>
       <c r="B277" s="2"/>
       <c r="C277" s="3"/>
-      <c r="D277" s="9"/>
+      <c r="D277" s="3"/>
+      <c r="E277" s="9"/>
     </row>
     <row r="278" spans="1:2">
       <c r="A278"/>
       <c r="B278" s="4"/>
     </row>
-    <row r="279" spans="1:4">
+    <row r="279" spans="1:5">
       <c r="A279"/>
       <c r="B279" s="2"/>
       <c r="C279" s="3"/>
-      <c r="D279" s="9"/>
-    </row>
-    <row r="280" spans="1:6">
+      <c r="D279" s="3"/>
+      <c r="E279" s="9"/>
+    </row>
+    <row r="280" spans="1:7">
       <c r="A280"/>
       <c r="B280" s="4"/>
       <c r="C280"/>
-      <c r="F280"/>
+      <c r="G280"/>
     </row>
     <row r="281" spans="1:3">
       <c r="A281"/>
@@ -2460,11 +2650,12 @@
       <c r="A282"/>
       <c r="B282" s="4"/>
     </row>
-    <row r="283" spans="1:4">
+    <row r="283" spans="1:5">
       <c r="A283"/>
       <c r="B283" s="2"/>
       <c r="C283" s="3"/>
-      <c r="D283" s="9"/>
+      <c r="D283" s="3"/>
+      <c r="E283" s="9"/>
     </row>
     <row r="284" spans="1:3">
       <c r="A284"/>
@@ -2476,45 +2667,47 @@
       <c r="B285" s="4"/>
       <c r="C285"/>
     </row>
-    <row r="286" spans="1:8">
+    <row r="286" spans="1:9">
       <c r="A286"/>
       <c r="B286" s="4"/>
       <c r="C286"/>
-      <c r="F286"/>
-      <c r="H286"/>
-    </row>
-    <row r="287" spans="1:6">
+      <c r="G286"/>
+      <c r="I286"/>
+    </row>
+    <row r="287" spans="1:7">
       <c r="A287"/>
       <c r="B287" s="4"/>
       <c r="C287"/>
-      <c r="F287"/>
+      <c r="G287"/>
     </row>
     <row r="288" spans="1:2">
       <c r="A288"/>
       <c r="B288" s="4"/>
     </row>
-    <row r="289" spans="1:4">
+    <row r="289" spans="1:5">
       <c r="A289"/>
       <c r="B289" s="2"/>
       <c r="C289" s="3"/>
-      <c r="D289" s="9"/>
-    </row>
-    <row r="290" spans="1:6">
+      <c r="D289" s="3"/>
+      <c r="E289" s="9"/>
+    </row>
+    <row r="290" spans="1:7">
       <c r="A290"/>
       <c r="B290" s="4"/>
       <c r="C290"/>
-      <c r="F290"/>
+      <c r="G290"/>
     </row>
     <row r="291" spans="1:3">
       <c r="A291"/>
       <c r="B291" s="4"/>
       <c r="C291"/>
     </row>
-    <row r="292" spans="1:4">
+    <row r="292" spans="1:5">
       <c r="A292"/>
       <c r="B292" s="5"/>
       <c r="C292" s="1"/>
-      <c r="D292" s="10"/>
+      <c r="D292" s="1"/>
+      <c r="E292" s="10"/>
     </row>
     <row r="293" spans="1:3">
       <c r="A293"/>
@@ -2540,111 +2733,120 @@
       <c r="A297"/>
       <c r="B297" s="4"/>
     </row>
-    <row r="298" spans="1:4">
+    <row r="298" spans="1:5">
       <c r="A298"/>
       <c r="B298" s="2"/>
       <c r="C298" s="3"/>
-      <c r="D298" s="9"/>
-    </row>
-    <row r="299" spans="1:6">
+      <c r="D298" s="3"/>
+      <c r="E298" s="9"/>
+    </row>
+    <row r="299" spans="1:7">
       <c r="A299"/>
       <c r="B299" s="4"/>
-      <c r="F299"/>
-    </row>
-    <row r="300" spans="1:4">
+      <c r="G299"/>
+    </row>
+    <row r="300" spans="1:5">
       <c r="A300"/>
       <c r="B300" s="5"/>
       <c r="C300" s="1"/>
-      <c r="D300" s="10"/>
+      <c r="D300" s="1"/>
+      <c r="E300" s="10"/>
     </row>
     <row r="301" spans="1:3">
       <c r="A301"/>
       <c r="B301" s="4"/>
       <c r="C301"/>
     </row>
-    <row r="302" spans="1:7">
+    <row r="302" spans="1:8">
       <c r="A302"/>
       <c r="B302" s="5"/>
       <c r="C302" s="1"/>
-      <c r="D302" s="10"/>
-      <c r="G302" s="8"/>
-    </row>
-    <row r="303" spans="1:7">
+      <c r="D302" s="1"/>
+      <c r="E302" s="10"/>
+      <c r="H302" s="8"/>
+    </row>
+    <row r="303" spans="1:8">
       <c r="A303"/>
       <c r="B303" s="4"/>
       <c r="C303"/>
-      <c r="G303" s="8"/>
+      <c r="H303" s="8"/>
     </row>
     <row r="304" spans="1:2">
       <c r="A304"/>
       <c r="B304" s="4"/>
     </row>
-    <row r="305" spans="1:7">
+    <row r="305" spans="1:8">
       <c r="A305"/>
       <c r="B305" s="2"/>
       <c r="C305" s="3"/>
-      <c r="D305" s="9"/>
-      <c r="G305" s="8"/>
-    </row>
-    <row r="306" spans="1:7">
+      <c r="D305" s="3"/>
+      <c r="E305" s="9"/>
+      <c r="H305" s="8"/>
+    </row>
+    <row r="306" spans="1:8">
       <c r="A306"/>
       <c r="B306" s="4"/>
-      <c r="G306" s="8"/>
-    </row>
-    <row r="307" spans="1:4">
+      <c r="H306" s="8"/>
+    </row>
+    <row r="307" spans="1:5">
       <c r="A307"/>
       <c r="B307" s="2"/>
       <c r="C307" s="3"/>
-      <c r="D307" s="9"/>
-    </row>
-    <row r="308" spans="1:5">
+      <c r="D307" s="3"/>
+      <c r="E307" s="9"/>
+    </row>
+    <row r="308" spans="1:6">
       <c r="A308"/>
       <c r="B308" s="4"/>
       <c r="C308"/>
-      <c r="E308" s="20"/>
-    </row>
-    <row r="309" spans="1:4">
+      <c r="F308" s="20"/>
+    </row>
+    <row r="309" spans="1:5">
       <c r="A309"/>
       <c r="B309" s="4"/>
-      <c r="D309"/>
-    </row>
-    <row r="310" spans="1:4">
+      <c r="E309"/>
+    </row>
+    <row r="310" spans="1:5">
       <c r="A310"/>
       <c r="B310" s="2"/>
       <c r="C310" s="3"/>
-      <c r="D310" s="9"/>
+      <c r="D310" s="3"/>
+      <c r="E310" s="9"/>
     </row>
     <row r="311" spans="1:2">
       <c r="A311"/>
       <c r="B311" s="4"/>
     </row>
-    <row r="312" spans="1:8">
+    <row r="312" spans="1:9">
       <c r="A312"/>
       <c r="B312" s="2"/>
       <c r="C312" s="3"/>
-      <c r="D312" s="9"/>
-      <c r="H312"/>
+      <c r="D312" s="3"/>
+      <c r="E312" s="9"/>
+      <c r="I312"/>
     </row>
     <row r="313" spans="1:2">
       <c r="A313"/>
       <c r="B313" s="4"/>
     </row>
-    <row r="314" spans="1:4">
+    <row r="314" spans="1:5">
       <c r="A314"/>
       <c r="B314" s="2"/>
       <c r="C314" s="3"/>
-      <c r="D314" s="9"/>
+      <c r="D314" s="3"/>
+      <c r="E314" s="9"/>
     </row>
     <row r="315" spans="1:2">
       <c r="A315"/>
       <c r="B315" s="4"/>
     </row>
-    <row r="316" spans="1:8">
+    <row r="316" spans="1:9">
       <c r="A316"/>
       <c r="B316" s="2"/>
       <c r="C316" s="3"/>
-      <c r="D316" s="9"/>
-      <c r="H316"/>
+      <c r="D316" s="3"/>
+      <c r="E316" s="9"/>
+      <c r="I316"/>
     </row>
     <row r="317" spans="1:3">
       <c r="A317"/>
@@ -2655,12 +2857,14 @@
       <c r="A318"/>
       <c r="B318" s="4"/>
     </row>
-    <row r="319" spans="1:9">
+    <row r="319" spans="1:10">
       <c r="A319"/>
       <c r="B319" s="2"/>
       <c r="C319" s="3"/>
-      <c r="D319" s="9"/>
+      <c r="D319" s="3"/>
+      <c r="E319" s="9"/>
       <c r="I319"/>
+      <c r="J319"/>
     </row>
     <row r="320" spans="1:3">
       <c r="A320"/>
@@ -2671,21 +2875,23 @@
       <c r="A321"/>
       <c r="B321" s="4"/>
     </row>
-    <row r="322" spans="1:4">
+    <row r="322" spans="1:5">
       <c r="A322"/>
       <c r="B322" s="2"/>
       <c r="C322" s="3"/>
-      <c r="D322" s="9"/>
+      <c r="D322" s="3"/>
+      <c r="E322" s="9"/>
     </row>
     <row r="323" spans="1:2">
       <c r="A323"/>
       <c r="B323" s="4"/>
     </row>
-    <row r="324" spans="1:4">
+    <row r="324" spans="1:5">
       <c r="A324"/>
       <c r="B324" s="2"/>
       <c r="C324" s="3"/>
-      <c r="D324" s="9"/>
+      <c r="D324" s="3"/>
+      <c r="E324" s="9"/>
     </row>
     <row r="325" spans="1:3">
       <c r="A325"/>
@@ -2696,11 +2902,12 @@
       <c r="A326"/>
       <c r="B326" s="4"/>
     </row>
-    <row r="327" spans="1:4">
+    <row r="327" spans="1:5">
       <c r="A327"/>
       <c r="B327" s="2"/>
       <c r="C327" s="3"/>
-      <c r="D327" s="9"/>
+      <c r="D327" s="3"/>
+      <c r="E327" s="9"/>
     </row>
     <row r="328" spans="1:3">
       <c r="A328"/>
@@ -2711,11 +2918,12 @@
       <c r="A329"/>
       <c r="B329" s="4"/>
     </row>
-    <row r="330" spans="1:4">
+    <row r="330" spans="1:5">
       <c r="A330"/>
       <c r="B330" s="2"/>
       <c r="C330" s="3"/>
-      <c r="D330" s="9"/>
+      <c r="D330" s="3"/>
+      <c r="E330" s="9"/>
     </row>
     <row r="331" spans="1:3">
       <c r="A331"/>
@@ -2731,21 +2939,23 @@
       <c r="A333"/>
       <c r="B333" s="4"/>
     </row>
-    <row r="334" spans="1:4">
+    <row r="334" spans="1:5">
       <c r="A334"/>
       <c r="B334" s="2"/>
       <c r="C334" s="3"/>
-      <c r="D334" s="9"/>
+      <c r="D334" s="3"/>
+      <c r="E334" s="9"/>
     </row>
     <row r="335" spans="1:2">
       <c r="A335"/>
       <c r="B335" s="4"/>
     </row>
-    <row r="336" spans="1:4">
+    <row r="336" spans="1:5">
       <c r="A336"/>
       <c r="B336" s="2"/>
       <c r="C336" s="3"/>
-      <c r="D336" s="9"/>
+      <c r="D336" s="3"/>
+      <c r="E336" s="9"/>
     </row>
     <row r="337" spans="1:3">
       <c r="A337"/>
@@ -2756,11 +2966,12 @@
       <c r="A338"/>
       <c r="B338" s="4"/>
     </row>
-    <row r="339" spans="1:4">
+    <row r="339" spans="1:5">
       <c r="A339"/>
       <c r="B339" s="2"/>
       <c r="C339" s="3"/>
-      <c r="D339" s="9"/>
+      <c r="D339" s="3"/>
+      <c r="E339" s="9"/>
     </row>
     <row r="340" spans="1:3">
       <c r="A340"/>
@@ -2771,146 +2982,167 @@
       <c r="A341"/>
       <c r="B341" s="4"/>
     </row>
-    <row r="342" spans="1:4">
+    <row r="342" spans="1:5">
       <c r="A342"/>
       <c r="B342" s="2"/>
       <c r="C342" s="3"/>
-      <c r="D342" s="9"/>
+      <c r="D342" s="3"/>
+      <c r="E342" s="9"/>
     </row>
     <row r="343" spans="1:2">
       <c r="A343"/>
       <c r="B343" s="4"/>
     </row>
-    <row r="344" spans="1:4">
+    <row r="344" spans="1:5">
       <c r="A344"/>
       <c r="B344" s="2"/>
       <c r="C344" s="3"/>
-      <c r="D344" s="9"/>
+      <c r="D344" s="3"/>
+      <c r="E344" s="9"/>
     </row>
     <row r="345" spans="1:2">
       <c r="A345"/>
       <c r="B345" s="4"/>
     </row>
-    <row r="346" spans="1:4">
+    <row r="346" spans="1:5">
       <c r="A346"/>
       <c r="B346" s="2"/>
       <c r="C346" s="3"/>
-      <c r="D346" s="9"/>
+      <c r="D346" s="3"/>
+      <c r="E346" s="9"/>
     </row>
     <row r="347" spans="1:2">
       <c r="A347"/>
       <c r="B347" s="4"/>
     </row>
-    <row r="348" spans="1:9">
+    <row r="348" spans="1:10">
       <c r="A348"/>
       <c r="B348" s="2"/>
       <c r="C348" s="3"/>
-      <c r="D348" s="9"/>
+      <c r="D348" s="3"/>
+      <c r="E348" s="9"/>
       <c r="I348"/>
-    </row>
-    <row r="349" spans="1:9">
+      <c r="J348"/>
+    </row>
+    <row r="349" spans="1:10">
       <c r="A349"/>
       <c r="B349" s="4"/>
       <c r="I349"/>
-    </row>
-    <row r="350" spans="1:9">
+      <c r="J349"/>
+    </row>
+    <row r="350" spans="1:10">
       <c r="A350"/>
       <c r="B350" s="4"/>
       <c r="I350"/>
+      <c r="J350"/>
     </row>
     <row r="351" spans="1:2">
       <c r="A351"/>
       <c r="B351" s="4"/>
     </row>
-    <row r="352" spans="1:9">
+    <row r="352" spans="1:10">
       <c r="A352"/>
       <c r="B352" s="2"/>
       <c r="C352" s="3"/>
-      <c r="D352" s="9"/>
+      <c r="D352" s="3"/>
+      <c r="E352" s="9"/>
       <c r="I352"/>
-    </row>
-    <row r="353" spans="1:9">
+      <c r="J352"/>
+    </row>
+    <row r="353" spans="1:10">
       <c r="A353"/>
       <c r="B353" s="4"/>
       <c r="I353"/>
+      <c r="J353"/>
     </row>
     <row r="354" spans="1:2">
       <c r="A354"/>
       <c r="B354" s="4"/>
     </row>
-    <row r="355" spans="1:9">
+    <row r="355" spans="1:10">
       <c r="A355"/>
       <c r="B355" s="2"/>
       <c r="C355" s="3"/>
-      <c r="D355" s="9"/>
+      <c r="D355" s="3"/>
+      <c r="E355" s="9"/>
       <c r="I355"/>
+      <c r="J355"/>
     </row>
     <row r="356" spans="1:2">
       <c r="A356"/>
       <c r="B356" s="4"/>
     </row>
-    <row r="357" spans="1:9">
+    <row r="357" spans="1:10">
       <c r="A357"/>
       <c r="B357" s="2"/>
       <c r="C357" s="3"/>
-      <c r="D357" s="9"/>
+      <c r="D357" s="3"/>
+      <c r="E357" s="9"/>
       <c r="I357"/>
-    </row>
-    <row r="358" spans="1:9">
+      <c r="J357"/>
+    </row>
+    <row r="358" spans="1:10">
       <c r="A358"/>
       <c r="B358" s="4"/>
       <c r="I358"/>
+      <c r="J358"/>
     </row>
     <row r="359" spans="1:2">
       <c r="A359"/>
       <c r="B359" s="4"/>
     </row>
-    <row r="360" spans="1:9">
+    <row r="360" spans="1:10">
       <c r="A360"/>
       <c r="B360" s="2"/>
       <c r="C360" s="3"/>
-      <c r="D360" s="9"/>
+      <c r="D360" s="3"/>
+      <c r="E360" s="9"/>
       <c r="I360"/>
+      <c r="J360"/>
     </row>
     <row r="361" spans="1:2">
       <c r="A361"/>
       <c r="B361" s="4"/>
     </row>
-    <row r="362" spans="1:4">
+    <row r="362" spans="1:5">
       <c r="A362"/>
       <c r="B362" s="2"/>
       <c r="C362" s="3"/>
-      <c r="D362" s="9"/>
+      <c r="D362" s="3"/>
+      <c r="E362" s="9"/>
     </row>
     <row r="363" spans="1:2">
       <c r="A363"/>
       <c r="B363" s="4"/>
     </row>
-    <row r="364" spans="1:4">
+    <row r="364" spans="1:5">
       <c r="A364"/>
       <c r="B364" s="2"/>
       <c r="C364" s="3"/>
-      <c r="D364" s="9"/>
+      <c r="D364" s="3"/>
+      <c r="E364" s="9"/>
     </row>
     <row r="365" spans="1:2">
       <c r="A365"/>
       <c r="B365" s="4"/>
     </row>
-    <row r="366" spans="1:4">
+    <row r="366" spans="1:5">
       <c r="A366"/>
       <c r="B366" s="2"/>
       <c r="C366" s="3"/>
-      <c r="D366" s="9"/>
+      <c r="D366" s="3"/>
+      <c r="E366" s="9"/>
     </row>
     <row r="367" spans="1:2">
       <c r="A367"/>
       <c r="B367" s="4"/>
     </row>
-    <row r="368" spans="1:4">
+    <row r="368" spans="1:5">
       <c r="A368"/>
       <c r="B368" s="2"/>
       <c r="C368" s="3"/>
-      <c r="D368" s="9"/>
+      <c r="D368" s="3"/>
+      <c r="E368" s="9"/>
     </row>
     <row r="369" spans="1:3">
       <c r="A369"/>
@@ -2921,31 +3153,34 @@
       <c r="A370"/>
       <c r="B370" s="4"/>
     </row>
-    <row r="371" spans="1:4">
+    <row r="371" spans="1:5">
       <c r="A371"/>
       <c r="B371" s="2"/>
       <c r="C371" s="3"/>
-      <c r="D371" s="9"/>
+      <c r="D371" s="3"/>
+      <c r="E371" s="9"/>
     </row>
     <row r="372" spans="1:2">
       <c r="A372"/>
       <c r="B372" s="4"/>
     </row>
-    <row r="373" spans="1:4">
+    <row r="373" spans="1:5">
       <c r="A373"/>
       <c r="B373" s="2"/>
       <c r="C373" s="3"/>
-      <c r="D373" s="9"/>
+      <c r="D373" s="3"/>
+      <c r="E373" s="9"/>
     </row>
     <row r="374" spans="1:2">
       <c r="A374"/>
       <c r="B374" s="4"/>
     </row>
-    <row r="375" spans="1:4">
+    <row r="375" spans="1:5">
       <c r="A375"/>
       <c r="B375" s="2"/>
       <c r="C375" s="3"/>
-      <c r="D375" s="9"/>
+      <c r="D375" s="3"/>
+      <c r="E375" s="9"/>
     </row>
     <row r="376" spans="1:3">
       <c r="A376"/>
@@ -2956,41 +3191,45 @@
       <c r="A377"/>
       <c r="B377" s="4"/>
     </row>
-    <row r="378" spans="1:4">
+    <row r="378" spans="1:5">
       <c r="A378"/>
       <c r="B378" s="2"/>
       <c r="C378" s="3"/>
-      <c r="D378" s="9"/>
+      <c r="D378" s="3"/>
+      <c r="E378" s="9"/>
     </row>
     <row r="379" spans="1:2">
       <c r="A379"/>
       <c r="B379" s="4"/>
     </row>
-    <row r="380" spans="1:4">
+    <row r="380" spans="1:5">
       <c r="A380"/>
       <c r="B380" s="2"/>
       <c r="C380" s="3"/>
-      <c r="D380" s="9"/>
+      <c r="D380" s="3"/>
+      <c r="E380" s="9"/>
     </row>
     <row r="381" spans="1:2">
       <c r="A381"/>
       <c r="B381" s="4"/>
     </row>
-    <row r="382" spans="1:4">
+    <row r="382" spans="1:5">
       <c r="A382"/>
       <c r="B382" s="2"/>
       <c r="C382" s="3"/>
-      <c r="D382" s="9"/>
+      <c r="D382" s="3"/>
+      <c r="E382" s="9"/>
     </row>
     <row r="383" spans="1:2">
       <c r="A383"/>
       <c r="B383" s="4"/>
     </row>
-    <row r="384" spans="1:4">
+    <row r="384" spans="1:5">
       <c r="A384"/>
       <c r="B384" s="2"/>
       <c r="C384" s="3"/>
-      <c r="D384" s="9"/>
+      <c r="D384" s="3"/>
+      <c r="E384" s="9"/>
     </row>
     <row r="385" spans="1:3">
       <c r="A385"/>
@@ -3011,100 +3250,117 @@
       <c r="A388"/>
       <c r="B388" s="4"/>
     </row>
-    <row r="389" spans="1:9">
+    <row r="389" spans="1:10">
       <c r="A389"/>
       <c r="B389" s="2"/>
       <c r="C389" s="9"/>
       <c r="D389" s="9"/>
+      <c r="E389" s="9"/>
       <c r="I389"/>
-    </row>
-    <row r="390" spans="1:9">
+      <c r="J389"/>
+    </row>
+    <row r="390" spans="1:10">
       <c r="A390"/>
       <c r="B390" s="4"/>
       <c r="C390"/>
       <c r="I390"/>
-    </row>
-    <row r="391" spans="1:9">
+      <c r="J390"/>
+    </row>
+    <row r="391" spans="1:10">
       <c r="A391"/>
       <c r="C391"/>
-      <c r="F391"/>
+      <c r="G391"/>
       <c r="I391"/>
-    </row>
-    <row r="392" spans="1:9">
+      <c r="J391"/>
+    </row>
+    <row r="392" spans="1:10">
       <c r="A392"/>
       <c r="B392" s="4"/>
       <c r="C392"/>
-      <c r="F392"/>
+      <c r="G392"/>
       <c r="I392"/>
+      <c r="J392"/>
     </row>
     <row r="393" spans="1:2">
       <c r="A393"/>
       <c r="B393" s="4"/>
     </row>
-    <row r="394" spans="1:9">
+    <row r="394" spans="1:10">
       <c r="A394"/>
       <c r="B394" s="2"/>
       <c r="C394" s="3"/>
-      <c r="D394" s="9"/>
+      <c r="D394" s="3"/>
+      <c r="E394" s="9"/>
       <c r="I394"/>
-    </row>
-    <row r="395" spans="1:9">
+      <c r="J394"/>
+    </row>
+    <row r="395" spans="1:10">
       <c r="A395"/>
       <c r="B395" s="4"/>
       <c r="C395"/>
       <c r="I395"/>
-    </row>
-    <row r="396" spans="1:9">
+      <c r="J395"/>
+    </row>
+    <row r="396" spans="1:10">
       <c r="A396"/>
       <c r="B396" s="4"/>
       <c r="C396"/>
-      <c r="F396"/>
+      <c r="G396"/>
       <c r="I396"/>
-    </row>
-    <row r="397" spans="1:9">
+      <c r="J396"/>
+    </row>
+    <row r="397" spans="1:10">
       <c r="A397"/>
       <c r="B397" s="2"/>
       <c r="C397" s="3"/>
-      <c r="D397" s="9"/>
+      <c r="D397" s="3"/>
+      <c r="E397" s="9"/>
       <c r="I397"/>
-    </row>
-    <row r="398" spans="1:9">
+      <c r="J397"/>
+    </row>
+    <row r="398" spans="1:10">
       <c r="A398"/>
       <c r="B398" s="4"/>
       <c r="C398"/>
       <c r="I398"/>
+      <c r="J398"/>
     </row>
     <row r="399" spans="1:2">
       <c r="A399"/>
       <c r="B399" s="4"/>
     </row>
-    <row r="400" spans="1:9">
+    <row r="400" spans="1:10">
       <c r="A400"/>
       <c r="B400" s="2"/>
       <c r="C400" s="3"/>
-      <c r="D400" s="9"/>
+      <c r="D400" s="3"/>
+      <c r="E400" s="9"/>
       <c r="I400"/>
+      <c r="J400"/>
     </row>
     <row r="401" spans="1:2">
       <c r="A401"/>
       <c r="B401" s="4"/>
     </row>
-    <row r="402" spans="1:9">
+    <row r="402" spans="1:10">
       <c r="A402"/>
       <c r="B402" s="2"/>
       <c r="C402" s="3"/>
-      <c r="D402" s="9"/>
+      <c r="D402" s="3"/>
+      <c r="E402" s="9"/>
       <c r="I402"/>
+      <c r="J402"/>
     </row>
     <row r="403" spans="1:2">
       <c r="A403"/>
       <c r="B403" s="4"/>
     </row>
-    <row r="404" spans="1:4">
+    <row r="404" spans="1:5">
       <c r="A404"/>
       <c r="B404" s="2"/>
       <c r="C404" s="3"/>
-      <c r="D404" s="9"/>
+      <c r="D404" s="3"/>
+      <c r="E404" s="9"/>
     </row>
     <row r="405" spans="1:3">
       <c r="A405"/>
@@ -3115,11 +3371,12 @@
       <c r="A406"/>
       <c r="B406" s="4"/>
     </row>
-    <row r="407" spans="1:4">
+    <row r="407" spans="1:5">
       <c r="A407"/>
       <c r="B407" s="2"/>
       <c r="C407" s="3"/>
-      <c r="D407" s="9"/>
+      <c r="D407" s="3"/>
+      <c r="E407" s="9"/>
     </row>
     <row r="408" spans="1:3">
       <c r="A408"/>
@@ -3135,130 +3392,152 @@
       <c r="A410"/>
       <c r="B410" s="4"/>
     </row>
-    <row r="411" spans="1:9">
+    <row r="411" spans="1:10">
       <c r="A411"/>
       <c r="B411" s="2"/>
       <c r="C411" s="3"/>
-      <c r="D411" s="9"/>
+      <c r="D411" s="3"/>
+      <c r="E411" s="9"/>
       <c r="I411"/>
+      <c r="J411"/>
     </row>
     <row r="412" spans="1:2">
       <c r="A412"/>
       <c r="B412" s="4"/>
     </row>
-    <row r="413" spans="1:9">
+    <row r="413" spans="1:10">
       <c r="A413"/>
       <c r="B413" s="2"/>
       <c r="C413" s="3"/>
-      <c r="D413" s="9"/>
+      <c r="D413" s="3"/>
+      <c r="E413" s="9"/>
       <c r="I413"/>
-    </row>
-    <row r="414" spans="1:9">
+      <c r="J413"/>
+    </row>
+    <row r="414" spans="1:10">
       <c r="A414"/>
       <c r="B414" s="4"/>
       <c r="I414"/>
-    </row>
-    <row r="415" spans="1:9">
+      <c r="J414"/>
+    </row>
+    <row r="415" spans="1:10">
       <c r="A415"/>
       <c r="B415" s="4"/>
       <c r="I415"/>
+      <c r="J415"/>
     </row>
     <row r="416" spans="1:2">
       <c r="A416"/>
       <c r="B416" s="4"/>
     </row>
-    <row r="417" spans="1:9">
+    <row r="417" spans="1:10">
       <c r="A417"/>
       <c r="B417" s="2"/>
       <c r="C417" s="3"/>
-      <c r="D417" s="9"/>
+      <c r="D417" s="3"/>
+      <c r="E417" s="9"/>
       <c r="I417"/>
-    </row>
-    <row r="418" spans="1:9">
+      <c r="J417"/>
+    </row>
+    <row r="418" spans="1:10">
       <c r="A418"/>
       <c r="B418" s="4"/>
-      <c r="F418"/>
+      <c r="G418"/>
       <c r="I418"/>
-    </row>
-    <row r="419" spans="1:9">
+      <c r="J418"/>
+    </row>
+    <row r="419" spans="1:10">
       <c r="A419"/>
       <c r="B419" s="4"/>
       <c r="I419"/>
+      <c r="J419"/>
     </row>
     <row r="420" spans="1:2">
       <c r="A420"/>
       <c r="B420" s="4"/>
     </row>
-    <row r="421" spans="1:9">
+    <row r="421" spans="1:10">
       <c r="A421"/>
       <c r="B421" s="2"/>
       <c r="C421" s="3"/>
-      <c r="D421" s="9"/>
+      <c r="D421" s="3"/>
+      <c r="E421" s="9"/>
       <c r="I421"/>
-    </row>
-    <row r="422" spans="1:4">
+      <c r="J421"/>
+    </row>
+    <row r="422" spans="1:5">
       <c r="A422"/>
       <c r="B422" s="5"/>
       <c r="C422" s="1"/>
-      <c r="D422" s="10"/>
+      <c r="D422" s="1"/>
+      <c r="E422" s="10"/>
     </row>
     <row r="423" spans="1:1">
       <c r="A423"/>
     </row>
-    <row r="424" spans="1:9">
+    <row r="424" spans="1:10">
       <c r="A424"/>
       <c r="B424" s="2"/>
       <c r="C424" s="3"/>
-      <c r="D424" s="9"/>
+      <c r="D424" s="3"/>
+      <c r="E424" s="9"/>
       <c r="I424"/>
-    </row>
-    <row r="425" spans="1:9">
+      <c r="J424"/>
+    </row>
+    <row r="425" spans="1:10">
       <c r="A425"/>
       <c r="B425" s="4"/>
-      <c r="F425"/>
+      <c r="G425"/>
       <c r="I425"/>
-    </row>
-    <row r="426" spans="1:4">
+      <c r="J425"/>
+    </row>
+    <row r="426" spans="1:5">
       <c r="A426"/>
       <c r="B426" s="5"/>
       <c r="C426" s="1"/>
-      <c r="D426" s="10"/>
+      <c r="D426" s="1"/>
+      <c r="E426" s="10"/>
     </row>
     <row r="427" spans="1:1">
       <c r="A427"/>
     </row>
-    <row r="428" spans="1:9">
+    <row r="428" spans="1:10">
       <c r="A428"/>
       <c r="B428" s="2"/>
       <c r="C428" s="3"/>
-      <c r="D428" s="9"/>
+      <c r="D428" s="3"/>
+      <c r="E428" s="9"/>
       <c r="I428"/>
+      <c r="J428"/>
     </row>
     <row r="429" spans="1:2">
       <c r="A429"/>
       <c r="B429" s="4"/>
     </row>
-    <row r="430" spans="1:4">
+    <row r="430" spans="1:5">
       <c r="A430"/>
       <c r="B430" s="2"/>
       <c r="C430" s="3"/>
-      <c r="D430" s="9"/>
+      <c r="D430" s="3"/>
+      <c r="E430" s="9"/>
     </row>
     <row r="431" spans="1:2">
       <c r="A431"/>
       <c r="B431" s="4"/>
     </row>
-    <row r="432" spans="1:4">
+    <row r="432" spans="1:5">
       <c r="A432"/>
       <c r="B432" s="2"/>
       <c r="C432" s="3"/>
-      <c r="D432" s="9"/>
-    </row>
-    <row r="433" spans="1:4">
+      <c r="D432" s="3"/>
+      <c r="E432" s="9"/>
+    </row>
+    <row r="433" spans="1:5">
       <c r="A433"/>
       <c r="B433" s="5"/>
       <c r="C433" s="1"/>
-      <c r="D433" s="10"/>
+      <c r="D433" s="1"/>
+      <c r="E433" s="10"/>
     </row>
     <row r="434" spans="1:2">
       <c r="A434"/>
@@ -3272,72 +3551,79 @@
       <c r="A436"/>
       <c r="B436" s="4"/>
     </row>
-    <row r="437" spans="1:4">
+    <row r="437" spans="1:5">
       <c r="A437"/>
       <c r="B437" s="2"/>
       <c r="C437" s="3"/>
-      <c r="D437" s="9"/>
+      <c r="D437" s="3"/>
+      <c r="E437" s="9"/>
     </row>
     <row r="438" spans="1:2">
       <c r="A438"/>
       <c r="B438" s="4"/>
     </row>
-    <row r="439" spans="1:4">
+    <row r="439" spans="1:5">
       <c r="A439"/>
       <c r="B439" s="2"/>
       <c r="C439" s="3"/>
-      <c r="D439" s="9"/>
+      <c r="D439" s="3"/>
+      <c r="E439" s="9"/>
     </row>
     <row r="440" spans="1:2">
       <c r="A440"/>
       <c r="B440" s="4"/>
     </row>
-    <row r="441" spans="1:4">
+    <row r="441" spans="1:5">
       <c r="A441"/>
       <c r="B441" s="2"/>
       <c r="C441" s="3"/>
-      <c r="D441" s="9"/>
+      <c r="D441" s="3"/>
+      <c r="E441" s="9"/>
     </row>
     <row r="442" spans="1:2">
       <c r="A442"/>
       <c r="B442" s="4"/>
     </row>
-    <row r="443" spans="1:4">
+    <row r="443" spans="1:5">
       <c r="A443"/>
       <c r="B443" s="2"/>
       <c r="C443" s="3"/>
-      <c r="D443" s="9"/>
+      <c r="D443" s="3"/>
+      <c r="E443" s="9"/>
     </row>
     <row r="444" spans="1:2">
       <c r="A444"/>
       <c r="B444" s="4"/>
     </row>
-    <row r="445" spans="1:4">
+    <row r="445" spans="1:5">
       <c r="A445"/>
       <c r="B445" s="2"/>
       <c r="C445" s="3"/>
-      <c r="D445" s="9"/>
+      <c r="D445" s="3"/>
+      <c r="E445" s="9"/>
     </row>
     <row r="446" spans="1:2">
       <c r="A446"/>
       <c r="B446" s="4"/>
     </row>
-    <row r="447" spans="1:4">
+    <row r="447" spans="1:5">
       <c r="A447"/>
       <c r="B447" s="2"/>
       <c r="C447" s="3"/>
-      <c r="D447" s="9"/>
+      <c r="D447" s="3"/>
+      <c r="E447" s="9"/>
     </row>
     <row r="448" spans="1:3">
       <c r="A448"/>
       <c r="B448" s="4"/>
       <c r="C448"/>
     </row>
-    <row r="449" spans="1:4">
+    <row r="449" spans="1:5">
       <c r="A449"/>
       <c r="B449" s="5"/>
       <c r="C449" s="1"/>
-      <c r="D449" s="10"/>
+      <c r="D449" s="1"/>
+      <c r="E449" s="10"/>
     </row>
     <row r="450" spans="1:3">
       <c r="A450"/>
@@ -3364,10 +3650,10 @@
       <c r="A456"/>
       <c r="C456"/>
     </row>
-    <row r="457" spans="1:4">
+    <row r="457" spans="1:5">
       <c r="A457"/>
       <c r="C457"/>
-      <c r="D457" s="9"/>
+      <c r="E457" s="9"/>
     </row>
     <row r="458" spans="1:1">
       <c r="A458"/>
@@ -3379,10 +3665,10 @@
     <row r="460" spans="1:1">
       <c r="A460"/>
     </row>
-    <row r="461" spans="1:4">
+    <row r="461" spans="1:5">
       <c r="A461"/>
       <c r="C461"/>
-      <c r="D461" s="9"/>
+      <c r="E461" s="9"/>
     </row>
     <row r="462" spans="1:1">
       <c r="A462"/>
@@ -3409,10 +3695,10 @@
     <row r="468" spans="1:1">
       <c r="A468"/>
     </row>
-    <row r="469" spans="1:4">
+    <row r="469" spans="1:5">
       <c r="A469"/>
       <c r="C469"/>
-      <c r="D469" s="9"/>
+      <c r="E469" s="9"/>
     </row>
     <row r="470" spans="1:1">
       <c r="A470"/>
@@ -3478,10 +3764,10 @@
     <row r="487" spans="1:1">
       <c r="A487"/>
     </row>
-    <row r="488" spans="1:4">
+    <row r="488" spans="1:5">
       <c r="A488"/>
       <c r="C488"/>
-      <c r="D488" s="9"/>
+      <c r="E488" s="9"/>
     </row>
     <row r="489" spans="1:1">
       <c r="A489"/>
@@ -3511,10 +3797,10 @@
     <row r="496" spans="1:1">
       <c r="A496"/>
     </row>
-    <row r="497" spans="1:4">
+    <row r="497" spans="1:5">
       <c r="A497"/>
       <c r="C497"/>
-      <c r="D497" s="9"/>
+      <c r="E497" s="9"/>
     </row>
     <row r="498" spans="1:1">
       <c r="A498"/>
@@ -3530,10 +3816,10 @@
     <row r="501" spans="1:1">
       <c r="A501"/>
     </row>
-    <row r="502" spans="1:4">
+    <row r="502" spans="1:5">
       <c r="A502"/>
       <c r="C502"/>
-      <c r="D502" s="9"/>
+      <c r="E502" s="9"/>
     </row>
     <row r="503" spans="1:3">
       <c r="A503"/>
@@ -3645,10 +3931,10 @@
     <row r="532" spans="1:1">
       <c r="A532"/>
     </row>
-    <row r="533" spans="1:6">
+    <row r="533" spans="1:7">
       <c r="A533"/>
       <c r="C533"/>
-      <c r="F533"/>
+      <c r="G533"/>
     </row>
     <row r="534" spans="1:3">
       <c r="A534"/>
@@ -3735,10 +4021,10 @@
       <c r="A556"/>
       <c r="C556"/>
     </row>
-    <row r="557" spans="1:8">
+    <row r="557" spans="1:9">
       <c r="A557"/>
       <c r="C557"/>
-      <c r="H557"/>
+      <c r="I557"/>
     </row>
     <row r="558" spans="1:1">
       <c r="A558"/>
@@ -3758,113 +4044,122 @@
     <row r="562" spans="1:1">
       <c r="A562"/>
     </row>
-    <row r="563" spans="1:7">
+    <row r="563" spans="1:8">
       <c r="A563"/>
       <c r="C563" s="15"/>
-      <c r="D563" s="16"/>
-      <c r="E563" s="21"/>
-      <c r="F563" s="16"/>
+      <c r="D563" s="15"/>
+      <c r="E563" s="16"/>
+      <c r="F563" s="21"/>
       <c r="G563" s="16"/>
-    </row>
-    <row r="564" spans="1:7">
+      <c r="H563" s="16"/>
+    </row>
+    <row r="564" spans="1:8">
       <c r="A564"/>
       <c r="C564" s="15"/>
-      <c r="D564" s="16"/>
-      <c r="E564" s="22"/>
-      <c r="F564" s="16"/>
+      <c r="D564" s="15"/>
+      <c r="E564" s="16"/>
+      <c r="F564" s="22"/>
       <c r="G564" s="16"/>
-    </row>
-    <row r="565" spans="1:7">
+      <c r="H564" s="16"/>
+    </row>
+    <row r="565" spans="1:8">
       <c r="A565"/>
       <c r="C565" s="15"/>
-      <c r="D565" s="16"/>
-      <c r="E565" s="22"/>
-      <c r="F565" s="16"/>
+      <c r="D565" s="15"/>
+      <c r="E565" s="16"/>
+      <c r="F565" s="22"/>
       <c r="G565" s="16"/>
-    </row>
-    <row r="566" spans="1:7">
+      <c r="H565" s="16"/>
+    </row>
+    <row r="566" spans="1:8">
       <c r="A566"/>
       <c r="C566" s="16"/>
       <c r="D566" s="16"/>
-      <c r="E566" s="22"/>
-      <c r="F566" s="16"/>
+      <c r="E566" s="16"/>
+      <c r="F566" s="22"/>
       <c r="G566" s="16"/>
-    </row>
-    <row r="567" spans="1:7">
+      <c r="H566" s="16"/>
+    </row>
+    <row r="567" spans="1:8">
       <c r="A567"/>
       <c r="C567" s="15"/>
-      <c r="D567" s="16"/>
-      <c r="E567" s="23"/>
-      <c r="F567" s="16"/>
+      <c r="D567" s="15"/>
+      <c r="E567" s="16"/>
+      <c r="F567" s="23"/>
       <c r="G567" s="16"/>
-    </row>
-    <row r="568" spans="1:7">
+      <c r="H567" s="16"/>
+    </row>
+    <row r="568" spans="1:8">
       <c r="A568"/>
       <c r="C568" s="16"/>
       <c r="D568" s="16"/>
-      <c r="E568" s="22"/>
-      <c r="F568" s="16"/>
+      <c r="E568" s="16"/>
+      <c r="F568" s="22"/>
       <c r="G568" s="16"/>
-    </row>
-    <row r="569" spans="1:7">
+      <c r="H568" s="16"/>
+    </row>
+    <row r="569" spans="1:8">
       <c r="A569"/>
       <c r="C569" s="15"/>
-      <c r="D569" s="16"/>
-      <c r="E569" s="23"/>
-      <c r="F569" s="16"/>
+      <c r="D569" s="15"/>
+      <c r="E569" s="16"/>
+      <c r="F569" s="23"/>
       <c r="G569" s="16"/>
-    </row>
-    <row r="570" spans="1:7">
+      <c r="H569" s="16"/>
+    </row>
+    <row r="570" spans="1:8">
       <c r="A570"/>
       <c r="C570" s="16"/>
       <c r="D570" s="16"/>
-      <c r="E570" s="22"/>
-      <c r="F570" s="16"/>
+      <c r="E570" s="16"/>
+      <c r="F570" s="22"/>
       <c r="G570" s="16"/>
-    </row>
-    <row r="571" spans="1:7">
+      <c r="H570" s="16"/>
+    </row>
+    <row r="571" spans="1:8">
       <c r="A571"/>
       <c r="C571" s="15"/>
-      <c r="D571" s="16"/>
-      <c r="E571" s="23"/>
-      <c r="F571" s="16"/>
+      <c r="D571" s="15"/>
+      <c r="E571" s="16"/>
+      <c r="F571" s="23"/>
       <c r="G571" s="16"/>
-    </row>
-    <row r="572" spans="1:7">
+      <c r="H571" s="16"/>
+    </row>
+    <row r="572" spans="1:8">
       <c r="A572"/>
-      <c r="D572"/>
-      <c r="G572"/>
-    </row>
-    <row r="573" spans="1:7">
+      <c r="E572"/>
+      <c r="H572"/>
+    </row>
+    <row r="573" spans="1:8">
       <c r="A573"/>
       <c r="C573"/>
-      <c r="D573"/>
-      <c r="G573" s="16"/>
-    </row>
-    <row r="574" spans="1:7">
+      <c r="E573"/>
+      <c r="H573" s="16"/>
+    </row>
+    <row r="574" spans="1:8">
       <c r="A574"/>
-      <c r="D574"/>
-      <c r="G574"/>
-    </row>
-    <row r="575" spans="1:7">
+      <c r="E574"/>
+      <c r="H574"/>
+    </row>
+    <row r="575" spans="1:8">
       <c r="A575"/>
       <c r="C575"/>
-      <c r="D575"/>
-      <c r="G575" s="16"/>
-    </row>
-    <row r="576" spans="1:7">
+      <c r="E575"/>
+      <c r="H575" s="16"/>
+    </row>
+    <row r="576" spans="1:8">
       <c r="A576"/>
-      <c r="D576"/>
-      <c r="G576"/>
+      <c r="E576"/>
+      <c r="H576"/>
     </row>
     <row r="577" spans="1:3">
       <c r="A577"/>
       <c r="C577"/>
     </row>
-    <row r="578" spans="1:7">
+    <row r="578" spans="1:8">
       <c r="A578"/>
       <c r="C578"/>
-      <c r="G578" s="16"/>
+      <c r="H578" s="16"/>
     </row>
     <row r="579" spans="1:1">
       <c r="A579"/>
@@ -3873,20 +4168,20 @@
       <c r="A580"/>
       <c r="C580"/>
     </row>
-    <row r="581" spans="1:7">
+    <row r="581" spans="1:8">
       <c r="A581"/>
-      <c r="D581"/>
-      <c r="G581"/>
-    </row>
-    <row r="582" spans="1:4">
+      <c r="E581"/>
+      <c r="H581"/>
+    </row>
+    <row r="582" spans="1:5">
       <c r="A582"/>
       <c r="C582"/>
-      <c r="D582"/>
-    </row>
-    <row r="583" spans="1:4">
+      <c r="E582"/>
+    </row>
+    <row r="583" spans="1:5">
       <c r="A583"/>
       <c r="C583"/>
-      <c r="D583"/>
+      <c r="E583"/>
     </row>
     <row r="584" spans="1:3">
       <c r="A584"/>
@@ -4019,7 +4314,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1645269141" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1666542496" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4028,14 +4323,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1645269141" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1645269141" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1666542496" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1666542496" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1645269141" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1666542496" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -4057,7 +4352,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1645269141" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1666542496" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4066,14 +4361,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1645269141" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1645269141" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1666542496" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1666542496" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1645269141" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1666542496" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -4095,7 +4390,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1645269141" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1666542496" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4104,14 +4399,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1645269141" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1645269141" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1666542496" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1666542496" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1645269141" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1666542496" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Rework of sql username and work of test database manager
</commit_message>
<xml_diff>
--- a/recount/test/test_files/excel_input_1.xlsx
+++ b/recount/test/test_files/excel_input_1.xlsx
@@ -15,17 +15,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1666542496" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1666542496" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1666542496" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1666542496"/>
+      <pm:revision xmlns:pm="smNativeData" day="1666639760" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1666639760" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1666639760" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1666639760"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>Reimbursement</t>
   </si>
   <si>
     <t>Category</t>
@@ -146,7 +143,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1666542496" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1666639760" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -161,7 +158,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1666542496" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1666639760" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -177,7 +174,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1666542496" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1666639760" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -192,7 +189,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1666542496" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1666639760" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="240" lang="default"/>
             <pm:ea face="Basic Roman" sz="240" lang="default"/>
@@ -201,7 +198,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,19 +229,8 @@
     <fill>
       <patternFill patternType="none"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1666542496" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -260,7 +246,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1666542496"/>
+          <pm:border xmlns:pm="smNativeData" id="1666639760"/>
         </ext>
       </extLst>
     </border>
@@ -279,7 +265,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1666542496">
+          <pm:border xmlns:pm="smNativeData" id="1666639760">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -300,7 +286,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1666542496">
+          <pm:border xmlns:pm="smNativeData" id="1666639760">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -322,7 +308,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1666542496">
+          <pm:border xmlns:pm="smNativeData" id="1666639760">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -343,7 +329,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1666542496">
+          <pm:border xmlns:pm="smNativeData" id="1666639760">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -364,7 +350,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1666542496">
+          <pm:border xmlns:pm="smNativeData" id="1666639760">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -386,7 +372,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1666542496">
+          <pm:border xmlns:pm="smNativeData" id="1666639760">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -409,7 +395,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1666542496">
+          <pm:border xmlns:pm="smNativeData" id="1666639760">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -431,28 +417,9 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1666542496">
+          <pm:border xmlns:pm="smNativeData" id="1666639760">
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1666542496"/>
         </ext>
       </extLst>
     </border>
@@ -516,10 +483,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1666542496" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1666639760" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1666542496" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1666639760" count="1">
         <pm:color name="Gris 20%" rgb="000000"/>
       </pm:colors>
     </ext>
@@ -786,7 +753,7 @@
   <dimension ref="A1:L624"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.553571" defaultRowHeight="15.40"/>
@@ -795,12 +762,11 @@
     <col min="3" max="4" width="16.107143" customWidth="1"/>
     <col min="5" max="5" width="51.330357" customWidth="1" style="8"/>
     <col min="6" max="6" width="12.000000" customWidth="1" style="18"/>
-    <col min="7" max="7" width="21.258929" customWidth="1"/>
-    <col min="8" max="8" width="36.330357" customWidth="1" style="14"/>
-    <col min="9" max="9" width="18.437500" customWidth="1"/>
-    <col min="10" max="10" width="27.357143" customWidth="1"/>
-    <col min="11" max="11" width="18.437500" customWidth="1"/>
-    <col min="12" max="12" width="14.000000" customWidth="1"/>
+    <col min="7" max="7" width="36.330357" customWidth="1" style="14"/>
+    <col min="8" max="8" width="18.437500" customWidth="1"/>
+    <col min="9" max="9" width="27.357143" customWidth="1"/>
+    <col min="10" max="10" width="18.437500" customWidth="1"/>
+    <col min="11" max="11" width="14.000000" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -822,19 +788,16 @@
       <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1"/>
+      <c r="J1"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="n">
@@ -844,27 +807,27 @@
         <v>246.550000000000011</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>12</v>
       </c>
       <c r="F2" s="18" t="n">
         <v>43678</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="G2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
         <v>13</v>
       </c>
       <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2"/>
+      <c r="J2"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="n">
@@ -874,21 +837,21 @@
         <v>545.230000000000018</v>
       </c>
       <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>18</v>
+      <c r="H3" t="s">
+        <v>13</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3"/>
+      <c r="J3"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="n">
@@ -898,25 +861,25 @@
         <v>30</v>
       </c>
       <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="F4" s="18" t="n">
         <v>43681</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="G4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
         <v>21</v>
       </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4"/>
-      <c r="L4" s="12"/>
+      <c r="J4"/>
+      <c r="K4" s="12"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="n">
@@ -928,17 +891,17 @@
       </c>
       <c r="C5"/>
       <c r="E5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="18" t="n">
         <v>43683</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="G5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5" t="s">
         <v>24</v>
-      </c>
-      <c r="I5"/>
-      <c r="J5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -949,25 +912,25 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="E6"/>
       <c r="F6" s="18" t="n">
         <v>43687</v>
       </c>
-      <c r="H6" s="14" t="s">
-        <v>28</v>
+      <c r="G6" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6"/>
+        <v>24</v>
+      </c>
+      <c r="J6"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="n">
@@ -978,13 +941,12 @@
       </c>
       <c r="C7"/>
       <c r="D7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7"/>
+      <c r="H7"/>
+      <c r="I7" t="s">
         <v>29</v>
-      </c>
-      <c r="E7"/>
-      <c r="G7"/>
-      <c r="I7"/>
-      <c r="J7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -995,18 +957,18 @@
         <v>30</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8"/>
       <c r="F8" s="18" t="n">
         <v>43692</v>
       </c>
-      <c r="H8" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8"/>
-      <c r="J8" t="s">
-        <v>25</v>
+      <c r="G8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8"/>
+      <c r="I8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1680,12 +1642,10 @@
     <row r="122" spans="1:7">
       <c r="A122"/>
       <c r="B122"/>
-      <c r="G122"/>
     </row>
     <row r="123" spans="1:7">
       <c r="A123"/>
       <c r="B123"/>
-      <c r="G123"/>
     </row>
     <row r="124" spans="1:4">
       <c r="A124"/>
@@ -1766,8 +1726,8 @@
       <c r="A136"/>
       <c r="B136" s="4"/>
       <c r="C136"/>
+      <c r="H136"/>
       <c r="I136"/>
-      <c r="J136"/>
     </row>
     <row r="137" spans="1:2">
       <c r="A137"/>
@@ -1859,14 +1819,14 @@
     <row r="151" spans="1:10">
       <c r="A151"/>
       <c r="B151" s="4"/>
+      <c r="H151"/>
       <c r="I151"/>
-      <c r="J151"/>
     </row>
     <row r="152" spans="1:10">
       <c r="A152"/>
       <c r="B152" s="4"/>
+      <c r="H152"/>
       <c r="I152"/>
-      <c r="J152"/>
     </row>
     <row r="153" spans="1:2">
       <c r="A153"/>
@@ -1939,8 +1899,8 @@
     <row r="165" spans="1:10">
       <c r="A165"/>
       <c r="B165" s="4"/>
+      <c r="H165"/>
       <c r="I165"/>
-      <c r="J165"/>
     </row>
     <row r="166" spans="1:2">
       <c r="A166"/>
@@ -1968,26 +1928,26 @@
       <c r="C170" s="3"/>
       <c r="D170" s="3"/>
       <c r="E170" s="9"/>
+      <c r="H170"/>
       <c r="I170"/>
-      <c r="J170"/>
     </row>
     <row r="171" spans="1:10">
       <c r="A171"/>
       <c r="B171" s="4"/>
+      <c r="H171"/>
       <c r="I171"/>
-      <c r="J171"/>
     </row>
     <row r="172" spans="1:10">
       <c r="A172"/>
       <c r="B172" s="4"/>
+      <c r="H172"/>
       <c r="I172"/>
-      <c r="J172"/>
     </row>
     <row r="173" spans="1:10">
       <c r="A173"/>
       <c r="B173" s="4"/>
+      <c r="H173"/>
       <c r="I173"/>
-      <c r="J173"/>
     </row>
     <row r="174" spans="1:5">
       <c r="A174"/>
@@ -1999,32 +1959,32 @@
     <row r="175" spans="1:10">
       <c r="A175"/>
       <c r="B175" s="4"/>
+      <c r="H175"/>
       <c r="I175"/>
-      <c r="J175"/>
     </row>
     <row r="176" spans="1:10">
       <c r="A176"/>
       <c r="B176" s="4"/>
+      <c r="H176"/>
       <c r="I176"/>
-      <c r="J176"/>
     </row>
     <row r="177" spans="1:10">
       <c r="A177"/>
       <c r="B177" s="4"/>
+      <c r="H177"/>
       <c r="I177"/>
-      <c r="J177"/>
     </row>
     <row r="178" spans="1:10">
       <c r="A178"/>
       <c r="B178" s="4"/>
+      <c r="H178"/>
       <c r="I178"/>
-      <c r="J178"/>
     </row>
     <row r="179" spans="1:10">
       <c r="A179"/>
       <c r="B179" s="4"/>
+      <c r="H179"/>
       <c r="I179"/>
-      <c r="J179"/>
     </row>
     <row r="180" spans="1:5">
       <c r="A180"/>
@@ -2039,20 +1999,20 @@
       <c r="C181" s="3"/>
       <c r="D181" s="3"/>
       <c r="E181" s="9"/>
+      <c r="H181"/>
       <c r="I181"/>
-      <c r="J181"/>
     </row>
     <row r="182" spans="1:10">
       <c r="A182"/>
       <c r="B182" s="4"/>
+      <c r="H182"/>
       <c r="I182"/>
-      <c r="J182"/>
     </row>
     <row r="183" spans="1:10">
       <c r="A183"/>
       <c r="B183" s="4"/>
+      <c r="H183"/>
       <c r="I183"/>
-      <c r="J183"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184"/>
@@ -2067,14 +2027,14 @@
       <c r="C185" s="3"/>
       <c r="D185" s="3"/>
       <c r="E185" s="9"/>
+      <c r="H185"/>
       <c r="I185"/>
-      <c r="J185"/>
     </row>
     <row r="186" spans="1:10">
       <c r="A186"/>
       <c r="B186" s="4"/>
+      <c r="H186"/>
       <c r="I186"/>
-      <c r="J186"/>
     </row>
     <row r="187" spans="1:5">
       <c r="A187"/>
@@ -2150,8 +2110,8 @@
     <row r="200" spans="1:10">
       <c r="A200"/>
       <c r="B200"/>
+      <c r="H200"/>
       <c r="I200"/>
-      <c r="J200"/>
     </row>
     <row r="201" spans="1:1">
       <c r="A201"/>
@@ -2171,8 +2131,8 @@
       <c r="C205" s="3"/>
       <c r="D205" s="3"/>
       <c r="E205" s="9"/>
+      <c r="H205"/>
       <c r="I205"/>
-      <c r="J205"/>
     </row>
     <row r="206" spans="1:5">
       <c r="A206"/>
@@ -2187,8 +2147,8 @@
       <c r="C207" s="3"/>
       <c r="D207" s="3"/>
       <c r="E207" s="9"/>
+      <c r="H207"/>
       <c r="I207"/>
-      <c r="J207"/>
     </row>
     <row r="208" spans="1:5">
       <c r="A208"/>
@@ -2203,8 +2163,8 @@
       <c r="C209" s="3"/>
       <c r="D209" s="3"/>
       <c r="E209" s="9"/>
+      <c r="H209"/>
       <c r="I209"/>
-      <c r="J209"/>
     </row>
     <row r="210" spans="1:5">
       <c r="A210"/>
@@ -2219,8 +2179,8 @@
       <c r="C211" s="3"/>
       <c r="D211" s="3"/>
       <c r="E211" s="9"/>
+      <c r="H211"/>
       <c r="I211"/>
-      <c r="J211"/>
     </row>
     <row r="212" spans="1:5">
       <c r="A212"/>
@@ -2372,30 +2332,29 @@
       <c r="C235" s="3"/>
       <c r="D235" s="3"/>
       <c r="E235" s="9"/>
+      <c r="H235"/>
       <c r="I235"/>
-      <c r="J235"/>
     </row>
     <row r="236" spans="1:10">
       <c r="A236"/>
       <c r="B236" s="4"/>
       <c r="C236"/>
+      <c r="H236"/>
       <c r="I236"/>
-      <c r="J236"/>
     </row>
     <row r="237" spans="1:10">
       <c r="A237"/>
       <c r="B237" s="4"/>
       <c r="C237"/>
-      <c r="G237"/>
+      <c r="H237"/>
       <c r="I237"/>
-      <c r="J237"/>
     </row>
     <row r="238" spans="1:10">
       <c r="A238"/>
       <c r="B238" s="4"/>
       <c r="C238"/>
+      <c r="H238"/>
       <c r="I238"/>
-      <c r="J238"/>
     </row>
     <row r="239" spans="1:5">
       <c r="A239"/>
@@ -2502,7 +2461,6 @@
       <c r="A256"/>
       <c r="B256" s="4"/>
       <c r="C256"/>
-      <c r="G256"/>
     </row>
     <row r="257" spans="1:3">
       <c r="A257"/>
@@ -2600,7 +2558,6 @@
       <c r="A273"/>
       <c r="B273" s="4"/>
       <c r="C273"/>
-      <c r="G273"/>
     </row>
     <row r="274" spans="1:2">
       <c r="A274"/>
@@ -2639,7 +2596,6 @@
       <c r="A280"/>
       <c r="B280" s="4"/>
       <c r="C280"/>
-      <c r="G280"/>
     </row>
     <row r="281" spans="1:3">
       <c r="A281"/>
@@ -2671,14 +2627,12 @@
       <c r="A286"/>
       <c r="B286" s="4"/>
       <c r="C286"/>
-      <c r="G286"/>
-      <c r="I286"/>
+      <c r="H286"/>
     </row>
     <row r="287" spans="1:7">
       <c r="A287"/>
       <c r="B287" s="4"/>
       <c r="C287"/>
-      <c r="G287"/>
     </row>
     <row r="288" spans="1:2">
       <c r="A288"/>
@@ -2695,7 +2649,6 @@
       <c r="A290"/>
       <c r="B290" s="4"/>
       <c r="C290"/>
-      <c r="G290"/>
     </row>
     <row r="291" spans="1:3">
       <c r="A291"/>
@@ -2743,7 +2696,6 @@
     <row r="299" spans="1:7">
       <c r="A299"/>
       <c r="B299" s="4"/>
-      <c r="G299"/>
     </row>
     <row r="300" spans="1:5">
       <c r="A300"/>
@@ -2763,13 +2715,13 @@
       <c r="C302" s="1"/>
       <c r="D302" s="1"/>
       <c r="E302" s="10"/>
-      <c r="H302" s="8"/>
+      <c r="G302" s="8"/>
     </row>
     <row r="303" spans="1:8">
       <c r="A303"/>
       <c r="B303" s="4"/>
       <c r="C303"/>
-      <c r="H303" s="8"/>
+      <c r="G303" s="8"/>
     </row>
     <row r="304" spans="1:2">
       <c r="A304"/>
@@ -2781,12 +2733,12 @@
       <c r="C305" s="3"/>
       <c r="D305" s="3"/>
       <c r="E305" s="9"/>
-      <c r="H305" s="8"/>
+      <c r="G305" s="8"/>
     </row>
     <row r="306" spans="1:8">
       <c r="A306"/>
       <c r="B306" s="4"/>
-      <c r="H306" s="8"/>
+      <c r="G306" s="8"/>
     </row>
     <row r="307" spans="1:5">
       <c r="A307"/>
@@ -2823,7 +2775,7 @@
       <c r="C312" s="3"/>
       <c r="D312" s="3"/>
       <c r="E312" s="9"/>
-      <c r="I312"/>
+      <c r="H312"/>
     </row>
     <row r="313" spans="1:2">
       <c r="A313"/>
@@ -2846,7 +2798,7 @@
       <c r="C316" s="3"/>
       <c r="D316" s="3"/>
       <c r="E316" s="9"/>
-      <c r="I316"/>
+      <c r="H316"/>
     </row>
     <row r="317" spans="1:3">
       <c r="A317"/>
@@ -2863,8 +2815,8 @@
       <c r="C319" s="3"/>
       <c r="D319" s="3"/>
       <c r="E319" s="9"/>
+      <c r="H319"/>
       <c r="I319"/>
-      <c r="J319"/>
     </row>
     <row r="320" spans="1:3">
       <c r="A320"/>
@@ -3021,20 +2973,20 @@
       <c r="C348" s="3"/>
       <c r="D348" s="3"/>
       <c r="E348" s="9"/>
+      <c r="H348"/>
       <c r="I348"/>
-      <c r="J348"/>
     </row>
     <row r="349" spans="1:10">
       <c r="A349"/>
       <c r="B349" s="4"/>
+      <c r="H349"/>
       <c r="I349"/>
-      <c r="J349"/>
     </row>
     <row r="350" spans="1:10">
       <c r="A350"/>
       <c r="B350" s="4"/>
+      <c r="H350"/>
       <c r="I350"/>
-      <c r="J350"/>
     </row>
     <row r="351" spans="1:2">
       <c r="A351"/>
@@ -3046,14 +2998,14 @@
       <c r="C352" s="3"/>
       <c r="D352" s="3"/>
       <c r="E352" s="9"/>
+      <c r="H352"/>
       <c r="I352"/>
-      <c r="J352"/>
     </row>
     <row r="353" spans="1:10">
       <c r="A353"/>
       <c r="B353" s="4"/>
+      <c r="H353"/>
       <c r="I353"/>
-      <c r="J353"/>
     </row>
     <row r="354" spans="1:2">
       <c r="A354"/>
@@ -3065,8 +3017,8 @@
       <c r="C355" s="3"/>
       <c r="D355" s="3"/>
       <c r="E355" s="9"/>
+      <c r="H355"/>
       <c r="I355"/>
-      <c r="J355"/>
     </row>
     <row r="356" spans="1:2">
       <c r="A356"/>
@@ -3078,14 +3030,14 @@
       <c r="C357" s="3"/>
       <c r="D357" s="3"/>
       <c r="E357" s="9"/>
+      <c r="H357"/>
       <c r="I357"/>
-      <c r="J357"/>
     </row>
     <row r="358" spans="1:10">
       <c r="A358"/>
       <c r="B358" s="4"/>
+      <c r="H358"/>
       <c r="I358"/>
-      <c r="J358"/>
     </row>
     <row r="359" spans="1:2">
       <c r="A359"/>
@@ -3097,8 +3049,8 @@
       <c r="C360" s="3"/>
       <c r="D360" s="3"/>
       <c r="E360" s="9"/>
+      <c r="H360"/>
       <c r="I360"/>
-      <c r="J360"/>
     </row>
     <row r="361" spans="1:2">
       <c r="A361"/>
@@ -3256,30 +3208,28 @@
       <c r="C389" s="9"/>
       <c r="D389" s="9"/>
       <c r="E389" s="9"/>
+      <c r="H389"/>
       <c r="I389"/>
-      <c r="J389"/>
     </row>
     <row r="390" spans="1:10">
       <c r="A390"/>
       <c r="B390" s="4"/>
       <c r="C390"/>
+      <c r="H390"/>
       <c r="I390"/>
-      <c r="J390"/>
     </row>
     <row r="391" spans="1:10">
       <c r="A391"/>
       <c r="C391"/>
-      <c r="G391"/>
+      <c r="H391"/>
       <c r="I391"/>
-      <c r="J391"/>
     </row>
     <row r="392" spans="1:10">
       <c r="A392"/>
       <c r="B392" s="4"/>
       <c r="C392"/>
-      <c r="G392"/>
+      <c r="H392"/>
       <c r="I392"/>
-      <c r="J392"/>
     </row>
     <row r="393" spans="1:2">
       <c r="A393"/>
@@ -3291,23 +3241,22 @@
       <c r="C394" s="3"/>
       <c r="D394" s="3"/>
       <c r="E394" s="9"/>
+      <c r="H394"/>
       <c r="I394"/>
-      <c r="J394"/>
     </row>
     <row r="395" spans="1:10">
       <c r="A395"/>
       <c r="B395" s="4"/>
       <c r="C395"/>
+      <c r="H395"/>
       <c r="I395"/>
-      <c r="J395"/>
     </row>
     <row r="396" spans="1:10">
       <c r="A396"/>
       <c r="B396" s="4"/>
       <c r="C396"/>
-      <c r="G396"/>
+      <c r="H396"/>
       <c r="I396"/>
-      <c r="J396"/>
     </row>
     <row r="397" spans="1:10">
       <c r="A397"/>
@@ -3315,15 +3264,15 @@
       <c r="C397" s="3"/>
       <c r="D397" s="3"/>
       <c r="E397" s="9"/>
+      <c r="H397"/>
       <c r="I397"/>
-      <c r="J397"/>
     </row>
     <row r="398" spans="1:10">
       <c r="A398"/>
       <c r="B398" s="4"/>
       <c r="C398"/>
+      <c r="H398"/>
       <c r="I398"/>
-      <c r="J398"/>
     </row>
     <row r="399" spans="1:2">
       <c r="A399"/>
@@ -3335,8 +3284,8 @@
       <c r="C400" s="3"/>
       <c r="D400" s="3"/>
       <c r="E400" s="9"/>
+      <c r="H400"/>
       <c r="I400"/>
-      <c r="J400"/>
     </row>
     <row r="401" spans="1:2">
       <c r="A401"/>
@@ -3348,8 +3297,8 @@
       <c r="C402" s="3"/>
       <c r="D402" s="3"/>
       <c r="E402" s="9"/>
+      <c r="H402"/>
       <c r="I402"/>
-      <c r="J402"/>
     </row>
     <row r="403" spans="1:2">
       <c r="A403"/>
@@ -3398,8 +3347,8 @@
       <c r="C411" s="3"/>
       <c r="D411" s="3"/>
       <c r="E411" s="9"/>
+      <c r="H411"/>
       <c r="I411"/>
-      <c r="J411"/>
     </row>
     <row r="412" spans="1:2">
       <c r="A412"/>
@@ -3411,20 +3360,20 @@
       <c r="C413" s="3"/>
       <c r="D413" s="3"/>
       <c r="E413" s="9"/>
+      <c r="H413"/>
       <c r="I413"/>
-      <c r="J413"/>
     </row>
     <row r="414" spans="1:10">
       <c r="A414"/>
       <c r="B414" s="4"/>
+      <c r="H414"/>
       <c r="I414"/>
-      <c r="J414"/>
     </row>
     <row r="415" spans="1:10">
       <c r="A415"/>
       <c r="B415" s="4"/>
+      <c r="H415"/>
       <c r="I415"/>
-      <c r="J415"/>
     </row>
     <row r="416" spans="1:2">
       <c r="A416"/>
@@ -3436,21 +3385,20 @@
       <c r="C417" s="3"/>
       <c r="D417" s="3"/>
       <c r="E417" s="9"/>
+      <c r="H417"/>
       <c r="I417"/>
-      <c r="J417"/>
     </row>
     <row r="418" spans="1:10">
       <c r="A418"/>
       <c r="B418" s="4"/>
-      <c r="G418"/>
+      <c r="H418"/>
       <c r="I418"/>
-      <c r="J418"/>
     </row>
     <row r="419" spans="1:10">
       <c r="A419"/>
       <c r="B419" s="4"/>
+      <c r="H419"/>
       <c r="I419"/>
-      <c r="J419"/>
     </row>
     <row r="420" spans="1:2">
       <c r="A420"/>
@@ -3462,8 +3410,8 @@
       <c r="C421" s="3"/>
       <c r="D421" s="3"/>
       <c r="E421" s="9"/>
+      <c r="H421"/>
       <c r="I421"/>
-      <c r="J421"/>
     </row>
     <row r="422" spans="1:5">
       <c r="A422"/>
@@ -3481,15 +3429,14 @@
       <c r="C424" s="3"/>
       <c r="D424" s="3"/>
       <c r="E424" s="9"/>
+      <c r="H424"/>
       <c r="I424"/>
-      <c r="J424"/>
     </row>
     <row r="425" spans="1:10">
       <c r="A425"/>
       <c r="B425" s="4"/>
-      <c r="G425"/>
+      <c r="H425"/>
       <c r="I425"/>
-      <c r="J425"/>
     </row>
     <row r="426" spans="1:5">
       <c r="A426"/>
@@ -3507,8 +3454,8 @@
       <c r="C428" s="3"/>
       <c r="D428" s="3"/>
       <c r="E428" s="9"/>
+      <c r="H428"/>
       <c r="I428"/>
-      <c r="J428"/>
     </row>
     <row r="429" spans="1:2">
       <c r="A429"/>
@@ -3934,7 +3881,6 @@
     <row r="533" spans="1:7">
       <c r="A533"/>
       <c r="C533"/>
-      <c r="G533"/>
     </row>
     <row r="534" spans="1:3">
       <c r="A534"/>
@@ -4024,7 +3970,7 @@
     <row r="557" spans="1:9">
       <c r="A557"/>
       <c r="C557"/>
-      <c r="I557"/>
+      <c r="H557"/>
     </row>
     <row r="558" spans="1:1">
       <c r="A558"/>
@@ -4051,7 +3997,6 @@
       <c r="E563" s="16"/>
       <c r="F563" s="21"/>
       <c r="G563" s="16"/>
-      <c r="H563" s="16"/>
     </row>
     <row r="564" spans="1:8">
       <c r="A564"/>
@@ -4060,7 +4005,6 @@
       <c r="E564" s="16"/>
       <c r="F564" s="22"/>
       <c r="G564" s="16"/>
-      <c r="H564" s="16"/>
     </row>
     <row r="565" spans="1:8">
       <c r="A565"/>
@@ -4069,7 +4013,6 @@
       <c r="E565" s="16"/>
       <c r="F565" s="22"/>
       <c r="G565" s="16"/>
-      <c r="H565" s="16"/>
     </row>
     <row r="566" spans="1:8">
       <c r="A566"/>
@@ -4078,7 +4021,6 @@
       <c r="E566" s="16"/>
       <c r="F566" s="22"/>
       <c r="G566" s="16"/>
-      <c r="H566" s="16"/>
     </row>
     <row r="567" spans="1:8">
       <c r="A567"/>
@@ -4087,7 +4029,6 @@
       <c r="E567" s="16"/>
       <c r="F567" s="23"/>
       <c r="G567" s="16"/>
-      <c r="H567" s="16"/>
     </row>
     <row r="568" spans="1:8">
       <c r="A568"/>
@@ -4096,7 +4037,6 @@
       <c r="E568" s="16"/>
       <c r="F568" s="22"/>
       <c r="G568" s="16"/>
-      <c r="H568" s="16"/>
     </row>
     <row r="569" spans="1:8">
       <c r="A569"/>
@@ -4105,7 +4045,6 @@
       <c r="E569" s="16"/>
       <c r="F569" s="23"/>
       <c r="G569" s="16"/>
-      <c r="H569" s="16"/>
     </row>
     <row r="570" spans="1:8">
       <c r="A570"/>
@@ -4114,7 +4053,6 @@
       <c r="E570" s="16"/>
       <c r="F570" s="22"/>
       <c r="G570" s="16"/>
-      <c r="H570" s="16"/>
     </row>
     <row r="571" spans="1:8">
       <c r="A571"/>
@@ -4123,34 +4061,33 @@
       <c r="E571" s="16"/>
       <c r="F571" s="23"/>
       <c r="G571" s="16"/>
-      <c r="H571" s="16"/>
     </row>
     <row r="572" spans="1:8">
       <c r="A572"/>
       <c r="E572"/>
-      <c r="H572"/>
+      <c r="G572"/>
     </row>
     <row r="573" spans="1:8">
       <c r="A573"/>
       <c r="C573"/>
       <c r="E573"/>
-      <c r="H573" s="16"/>
+      <c r="G573" s="16"/>
     </row>
     <row r="574" spans="1:8">
       <c r="A574"/>
       <c r="E574"/>
-      <c r="H574"/>
+      <c r="G574"/>
     </row>
     <row r="575" spans="1:8">
       <c r="A575"/>
       <c r="C575"/>
       <c r="E575"/>
-      <c r="H575" s="16"/>
+      <c r="G575" s="16"/>
     </row>
     <row r="576" spans="1:8">
       <c r="A576"/>
       <c r="E576"/>
-      <c r="H576"/>
+      <c r="G576"/>
     </row>
     <row r="577" spans="1:3">
       <c r="A577"/>
@@ -4159,7 +4096,7 @@
     <row r="578" spans="1:8">
       <c r="A578"/>
       <c r="C578"/>
-      <c r="H578" s="16"/>
+      <c r="G578" s="16"/>
     </row>
     <row r="579" spans="1:1">
       <c r="A579"/>
@@ -4171,7 +4108,7 @@
     <row r="581" spans="1:8">
       <c r="A581"/>
       <c r="E581"/>
-      <c r="H581"/>
+      <c r="G581"/>
     </row>
     <row r="582" spans="1:5">
       <c r="A582"/>
@@ -4314,7 +4251,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1666542496" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1666639760" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4323,14 +4260,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1666542496" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1666542496" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1666639760" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1666639760" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1666542496" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1666639760" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -4352,7 +4289,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1666542496" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1666639760" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4361,14 +4298,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1666542496" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1666542496" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1666639760" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1666639760" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1666542496" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1666639760" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -4390,7 +4327,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1666542496" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1666639760" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4399,14 +4336,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1666542496" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1666542496" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1666639760" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1666639760" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1666542496" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1666639760" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>